<commit_message>
ran E5 CRM test to see variability from probe 20210228 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D010E53-BAF7-42CF-8D68-C3F8AB4698FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D46D67-77B6-4A23-B2B3-6CB76A38F2F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -52,12 +52,15 @@
   <si>
     <t>CRM opened 20210216</t>
   </si>
+  <si>
+    <t>CRM opened 20210228</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +191,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -891,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +952,176 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20210228</v>
+      </c>
+      <c r="B3">
+        <v>2211.1392636523301</v>
+      </c>
+      <c r="C3">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">100*(B3-C3)/C3</f>
+        <v>-1.0264108263246032</v>
+      </c>
+      <c r="E3">
+        <v>141</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20210228</v>
+      </c>
+      <c r="B4">
+        <v>2213.5992626297498</v>
+      </c>
+      <c r="C4">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>-0.91629793919843106</v>
+      </c>
+      <c r="E4">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20210228</v>
+      </c>
+      <c r="B5">
+        <v>2218.8110320871701</v>
+      </c>
+      <c r="C5">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-0.68301207718782442</v>
+      </c>
+      <c r="E5">
+        <v>141</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20210228</v>
+      </c>
+      <c r="B6">
+        <v>2208.8304250821302</v>
+      </c>
+      <c r="C6">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-1.1297575688259525</v>
+      </c>
+      <c r="E6">
+        <v>141</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20210228</v>
+      </c>
+      <c r="B7">
+        <v>2203.4973775284002</v>
+      </c>
+      <c r="C7">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-1.3684720027393935</v>
+      </c>
+      <c r="E7">
+        <v>141</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20210228</v>
+      </c>
+      <c r="B8">
+        <v>2213.3549756320699</v>
+      </c>
+      <c r="C8">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.9272325561835687</v>
+      </c>
+      <c r="E8">
+        <v>141</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20210228</v>
+      </c>
+      <c r="B9">
+        <v>2230.9452295190799</v>
+      </c>
+      <c r="C9">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.13986896027967938</v>
+      </c>
+      <c r="E9">
+        <v>141</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20210228</v>
+      </c>
+      <c r="B10">
+        <v>2222.5457646464001</v>
+      </c>
+      <c r="C10">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.515840387883998</v>
+      </c>
+      <c r="E10">
+        <v>141</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added CRM accuracy data for 0221 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D46D67-77B6-4A23-B2B3-6CB76A38F2F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B4B0FBB-8E56-0B46-B8A0-395F6535BD08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="1180" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>CRM opened 20210228</t>
+  </si>
+  <si>
+    <t>CRM opened 20210221</t>
   </si>
 </sst>
 </file>
@@ -900,18 +903,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -952,171 +956,192 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20210228</v>
+        <v>20210221</v>
       </c>
       <c r="B3">
-        <v>2211.1392636523301</v>
+        <v>2215.5540000000001</v>
       </c>
       <c r="C3">
         <v>2234.0700000000002</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D10" si="0">100*(B3-C3)/C3</f>
-        <v>-1.0264108263246032</v>
+        <f>100*(B3-C3)/C3</f>
+        <v>-0.82880124615612205</v>
       </c>
       <c r="E3">
         <v>141</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210228</v>
       </c>
       <c r="B4">
-        <v>2213.5992626297498</v>
+        <v>2211.1392636523301</v>
       </c>
       <c r="C4">
         <v>2234.0700000000002</v>
       </c>
       <c r="D4">
+        <f t="shared" ref="D4:D11" si="0">100*(B4-C4)/C4</f>
+        <v>-1.0264108263246032</v>
+      </c>
+      <c r="E4">
+        <v>141</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20210228</v>
+      </c>
+      <c r="B5">
+        <v>2213.5992626297498</v>
+      </c>
+      <c r="C5">
+        <v>2234.0700000000002</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>-0.91629793919843106</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>141</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>20210228</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>2218.8110320871701</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>-0.68301207718782442</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>141</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>20210228</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2208.8304250821302</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>-1.1297575688259525</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>141</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>20210228</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>2203.4973775284002</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>-1.3684720027393935</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>141</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>20210228</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>2213.3549756320699</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>-0.9272325561835687</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>141</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>20210228</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>2230.9452295190799</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>-0.13986896027967938</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>141</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>20210228</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>2222.5457646464001</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>-0.515840387883998</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>141</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added CRM data from 0221 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412F02C5-71EF-4746-95F2-9E3645FDE1BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D232FC-F411-4C4D-8FA3-43562801F69F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1180" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -906,7 +906,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
CRM test with new probe 0314 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D232FC-F411-4C4D-8FA3-43562801F69F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4B51A9-7E4D-4B54-AD3D-059050FB9A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1180" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="1410" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -905,17 +905,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -956,7 +956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -998,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20210228</v>
       </c>

</xml_diff>

<commit_message>
updated CRM accuracy data sheet
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4B51A9-7E4D-4B54-AD3D-059050FB9A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B43F65-2745-CA46-AB7C-D1073870194E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1410" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4000" yWindow="1420" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -903,19 +903,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -956,7 +956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -998,7 +998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1142,6 +1142,174 @@
         <v>141</v>
       </c>
       <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20210314</v>
+      </c>
+      <c r="B12">
+        <v>2182.6919702618002</v>
+      </c>
+      <c r="C12">
+        <v>2235.0700000000002</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D19" si="1">100*(B12-C12)/C12</f>
+        <v>-2.3434626091442317</v>
+      </c>
+      <c r="E12">
+        <v>141</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>20210314</v>
+      </c>
+      <c r="B13">
+        <v>2183.0707049272701</v>
+      </c>
+      <c r="C13">
+        <v>2236.0700000000002</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>-2.370198387024113</v>
+      </c>
+      <c r="E13">
+        <v>141</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>20210314</v>
+      </c>
+      <c r="B14">
+        <v>2179.9893168764502</v>
+      </c>
+      <c r="C14">
+        <v>2237.0700000000002</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-2.5515823431340987</v>
+      </c>
+      <c r="E14">
+        <v>141</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>20210314</v>
+      </c>
+      <c r="B15">
+        <v>2180.1189155137999</v>
+      </c>
+      <c r="C15">
+        <v>2238.0700000000002</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-2.5893329737765223</v>
+      </c>
+      <c r="E15">
+        <v>141</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20210314</v>
+      </c>
+      <c r="B16">
+        <v>2194.2628893932401</v>
+      </c>
+      <c r="C16">
+        <v>2239.0700000000002</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>-2.0011482716824411</v>
+      </c>
+      <c r="E16">
+        <v>141</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>20210314</v>
+      </c>
+      <c r="B17">
+        <v>2194.8087986166001</v>
+      </c>
+      <c r="C17">
+        <v>2240.0700000000002</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>-2.0205262060292766</v>
+      </c>
+      <c r="E17">
+        <v>141</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>20210314</v>
+      </c>
+      <c r="B18">
+        <v>2192.1340883392099</v>
+      </c>
+      <c r="C18">
+        <v>2241.0700000000002</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>-2.1835958564788349</v>
+      </c>
+      <c r="E18">
+        <v>141</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>20210314</v>
+      </c>
+      <c r="B19">
+        <v>2192.25361055657</v>
+      </c>
+      <c r="C19">
+        <v>2242.0700000000002</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>-2.2218926903901361</v>
+      </c>
+      <c r="E19">
+        <v>141</v>
+      </c>
+      <c r="F19" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
opened new CRM for values dmb 0314
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B43F65-2745-CA46-AB7C-D1073870194E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D61C07-6E03-47D1-A964-9AD3828F1CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="1420" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3990" yWindow="1410" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>CRM opened 20210221</t>
+  </si>
+  <si>
+    <t>CRM opened 20210314</t>
   </si>
 </sst>
 </file>
@@ -903,19 +906,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -956,7 +959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -977,7 +980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>2235.0700000000002</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D19" si="1">100*(B12-C12)/C12</f>
+        <f t="shared" ref="D12:D23" si="1">100*(B12-C12)/C12</f>
         <v>-2.3434626091442317</v>
       </c>
       <c r="E12">
@@ -1166,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1313,8 +1316,93 @@
         <v>7</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20210314</v>
+      </c>
+      <c r="B20">
+        <v>2205.7312106719601</v>
+      </c>
+      <c r="C20">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>-0.84239343879844331</v>
+      </c>
+      <c r="E20">
+        <v>180</v>
+      </c>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20210314</v>
+      </c>
+      <c r="B21">
+        <v>2194.00552102248</v>
+      </c>
+      <c r="C21">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>-1.3695162882628122</v>
+      </c>
+      <c r="E21">
+        <v>180</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20210314</v>
+      </c>
+      <c r="B22">
+        <v>2192.0447529285698</v>
+      </c>
+      <c r="C22">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>-1.4576616934114655</v>
+      </c>
+      <c r="E22">
+        <v>180</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20210314</v>
+      </c>
+      <c r="B23">
+        <v>2196.3789375564002</v>
+      </c>
+      <c r="C23">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>-1.2628204670595531</v>
+      </c>
+      <c r="E23">
+        <v>180</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edited CRM Accuracy Data sheet for correct 141 batch CRM
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D61C07-6E03-47D1-A964-9AD3828F1CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72A008-0C3D-8A43-843F-593EF44027BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1410" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7620" yWindow="500" windowWidth="16420" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -908,17 +908,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -959,7 +959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -980,7 +980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1156,11 +1156,11 @@
         <v>2182.6919702618002</v>
       </c>
       <c r="C12">
-        <v>2235.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D23" si="1">100*(B12-C12)/C12</f>
-        <v>-2.3434626091442317</v>
+        <v>-2.2997502199214876</v>
       </c>
       <c r="E12">
         <v>141</v>
@@ -1169,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1177,11 +1177,11 @@
         <v>2183.0707049272701</v>
       </c>
       <c r="C13">
-        <v>2236.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>-2.370198387024113</v>
+        <v>-2.2827975431714354</v>
       </c>
       <c r="E13">
         <v>141</v>
@@ -1190,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1198,11 +1198,11 @@
         <v>2179.9893168764502</v>
       </c>
       <c r="C14">
-        <v>2237.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>-2.5515823431340987</v>
+        <v>-2.4207246471037158</v>
       </c>
       <c r="E14">
         <v>141</v>
@@ -1211,7 +1211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1219,11 +1219,11 @@
         <v>2180.1189155137999</v>
       </c>
       <c r="C15">
-        <v>2238.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>-2.5893329737765223</v>
+        <v>-2.4149236365109514</v>
       </c>
       <c r="E15">
         <v>141</v>
@@ -1232,7 +1232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1240,11 +1240,11 @@
         <v>2194.2628893932401</v>
       </c>
       <c r="C16">
-        <v>2239.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>-2.0011482716824411</v>
+        <v>-1.7818202028924801</v>
       </c>
       <c r="E16">
         <v>141</v>
@@ -1253,7 +1253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1261,11 +1261,11 @@
         <v>2194.8087986166001</v>
       </c>
       <c r="C17">
-        <v>2240.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>-2.0205262060292766</v>
+        <v>-1.7573845664370418</v>
       </c>
       <c r="E17">
         <v>141</v>
@@ -1274,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1282,11 +1282,11 @@
         <v>2192.1340883392099</v>
       </c>
       <c r="C18">
-        <v>2241.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>-2.1835958564788349</v>
+        <v>-1.8771082222486413</v>
       </c>
       <c r="E18">
         <v>141</v>
@@ -1295,7 +1295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1303,11 +1303,11 @@
         <v>2192.25361055657</v>
       </c>
       <c r="C19">
-        <v>2242.0700000000002</v>
+        <v>2234.0700000000002</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>-2.2218926903901361</v>
+        <v>-1.8717582458665181</v>
       </c>
       <c r="E19">
         <v>141</v>
@@ -1316,7 +1316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20210314</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20210314</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20210314</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20210314</v>
       </c>

</xml_diff>

<commit_message>
replaced titrant/acid, same A16 batch number, solved all issues, ran three blue tank samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72A008-0C3D-8A43-843F-593EF44027BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A693DCD-E7F9-4F3C-B247-7ECAF211BC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="500" windowWidth="16420" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -906,19 +906,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -959,7 +959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -980,7 +980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20210314</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20210314</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20210314</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20210314</v>
       </c>
@@ -1397,6 +1397,132 @@
         <v>180</v>
       </c>
       <c r="F23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20210328</v>
+      </c>
+      <c r="B24">
+        <v>2766.9919084923999</v>
+      </c>
+      <c r="C24">
+        <v>2225.4699999999998</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D29" si="2">100*(B24-C24)/C24</f>
+        <v>24.332923314733524</v>
+      </c>
+      <c r="E24">
+        <v>180</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20210328</v>
+      </c>
+      <c r="B25">
+        <v>2226.22004515256</v>
+      </c>
+      <c r="C25">
+        <v>2226.4699999999998</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>-1.1226508663479276E-2</v>
+      </c>
+      <c r="E25">
+        <v>180</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20210328</v>
+      </c>
+      <c r="B26">
+        <v>2224.4256267383998</v>
+      </c>
+      <c r="C26">
+        <v>2227.4699999999998</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>-0.13667404102411965</v>
+      </c>
+      <c r="E26">
+        <v>180</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20210328</v>
+      </c>
+      <c r="B27">
+        <v>2224.2019706982401</v>
+      </c>
+      <c r="C27">
+        <v>2228.4699999999998</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>-0.19152285208056313</v>
+      </c>
+      <c r="E27">
+        <v>180</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20210328</v>
+      </c>
+      <c r="B28">
+        <v>2225.54963650217</v>
+      </c>
+      <c r="C28">
+        <v>2229.4699999999998</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>-0.17584284596024347</v>
+      </c>
+      <c r="E28">
+        <v>180</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20210328</v>
+      </c>
+      <c r="B29">
+        <v>2228.2924875591002</v>
+      </c>
+      <c r="C29">
+        <v>2230.4699999999998</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>-9.7625721973377405E-2</v>
+      </c>
+      <c r="E29">
+        <v>180</v>
+      </c>
+      <c r="F29" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CRM and pH calibration run 0404 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A693DCD-E7F9-4F3C-B247-7ECAF211BC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6CDB79-86A4-4CFD-A317-A350FB317320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="720" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>CRM opened 20210314</t>
+  </si>
+  <si>
+    <t>CRM opened 20210404</t>
   </si>
 </sst>
 </file>
@@ -906,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,6 +1529,27 @@
         <v>9</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20210404</v>
+      </c>
+      <c r="B30">
+        <v>2272.8870000000002</v>
+      </c>
+      <c r="C30">
+        <v>2231.4699999999998</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30" si="3">100*(B30-C30)/C30</f>
+        <v>1.8560410850246867</v>
+      </c>
+      <c r="E30">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edited CRM batch values for correct accuracy calculation
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6CDB79-86A4-4CFD-A317-A350FB317320}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211B64A1-F4B9-D943-B511-494249EED598}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="720" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5280" yWindow="720" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -909,19 +909,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -962,7 +962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -983,7 +983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20210314</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20210314</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20210314</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20210314</v>
       </c>
@@ -1403,19 +1403,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20210328</v>
       </c>
       <c r="B24">
-        <v>2766.9919084923999</v>
+        <v>2226.22004515256</v>
       </c>
       <c r="C24">
-        <v>2225.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D29" si="2">100*(B24-C24)/C24</f>
-        <v>24.332923314733524</v>
+        <f t="shared" ref="D24:D28" si="2">100*(B24-C24)/C24</f>
+        <v>7.8672454677304396E-2</v>
       </c>
       <c r="E24">
         <v>180</v>
@@ -1424,19 +1424,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20210328</v>
       </c>
       <c r="B25">
-        <v>2226.22004515256</v>
+        <v>2224.4256267383998</v>
       </c>
       <c r="C25">
-        <v>2226.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>-1.1226508663479276E-2</v>
+        <v>-1.9947790529860109E-3</v>
       </c>
       <c r="E25">
         <v>180</v>
@@ -1445,19 +1445,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20210328</v>
       </c>
       <c r="B26">
-        <v>2224.4256267383998</v>
+        <v>2224.2019706982401</v>
       </c>
       <c r="C26">
-        <v>2227.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>-0.13667404102411965</v>
+        <v>-1.2049130883299172E-2</v>
       </c>
       <c r="E26">
         <v>180</v>
@@ -1466,19 +1466,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20210328</v>
       </c>
       <c r="B27">
-        <v>2224.2019706982401</v>
+        <v>2225.54963650217</v>
       </c>
       <c r="C27">
-        <v>2228.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D27">
         <f t="shared" si="2"/>
-        <v>-0.19152285208056313</v>
+        <v>4.8534549900432933E-2</v>
       </c>
       <c r="E27">
         <v>180</v>
@@ -1487,19 +1487,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20210328</v>
       </c>
       <c r="B28">
-        <v>2225.54963650217</v>
+        <v>2228.2924875591002</v>
       </c>
       <c r="C28">
-        <v>2229.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D28">
         <f t="shared" si="2"/>
-        <v>-0.17584284596024347</v>
+        <v>0.17183812589517547</v>
       </c>
       <c r="E28">
         <v>180</v>
@@ -1508,45 +1508,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>20210328</v>
+        <v>20210404</v>
       </c>
       <c r="B29">
-        <v>2228.2924875591002</v>
+        <v>2272.8870000000002</v>
       </c>
       <c r="C29">
-        <v>2230.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D29">
-        <f t="shared" si="2"/>
-        <v>-9.7625721973377405E-2</v>
+        <f t="shared" ref="D29" si="3">100*(B29-C29)/C29</f>
+        <v>2.1765634061147319</v>
       </c>
       <c r="E29">
         <v>180</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>20210404</v>
-      </c>
-      <c r="B30">
-        <v>2272.8870000000002</v>
-      </c>
-      <c r="C30">
-        <v>2231.4699999999998</v>
-      </c>
-      <c r="D30">
-        <f t="shared" ref="D30" si="3">100*(B30-C30)/C30</f>
-        <v>1.8560410850246867</v>
-      </c>
-      <c r="E30">
-        <v>180</v>
-      </c>
-      <c r="F30" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
polyp bailout tanks CRM accuracy data dmb 0418
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211B64A1-F4B9-D943-B511-494249EED598}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E32BE83-0933-4E63-9108-78F6FD33FAA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="720" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="840" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>CRM opened 20210404</t>
+  </si>
+  <si>
+    <t>CRM opened 20210418</t>
   </si>
 </sst>
 </file>
@@ -909,19 +912,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -941,7 +944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -962,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -983,7 +986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1172,7 +1175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1319,7 +1322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20210314</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20210314</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20210314</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20210314</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20210328</v>
       </c>
@@ -1424,7 +1427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20210328</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20210328</v>
       </c>
@@ -1466,7 +1469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20210328</v>
       </c>
@@ -1487,7 +1490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20210328</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>20210404</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29" si="3">100*(B29-C29)/C29</f>
+        <f t="shared" ref="D29:D30" si="3">100*(B29-C29)/C29</f>
         <v>2.1765634061147319</v>
       </c>
       <c r="E29">
@@ -1527,6 +1530,27 @@
       </c>
       <c r="F29" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20210418</v>
+      </c>
+      <c r="B30">
+        <v>2218.2559999999999</v>
+      </c>
+      <c r="C30">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>-0.27934744006437229</v>
+      </c>
+      <c r="E30">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran triplicate titrations for blue tank polyp bailout dmb 0428
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E32BE83-0933-4E63-9108-78F6FD33FAA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819E23B-AD51-4465-B4BA-7827ED93ADF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="840" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="945" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,6 +1553,27 @@
         <v>11</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20210428</v>
+      </c>
+      <c r="B31">
+        <v>2223.7829999999999</v>
+      </c>
+      <c r="C31">
+        <v>2225.4699999999998</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31" si="4">100*(B31-C31)/C31</f>
+        <v>-7.5804212143947045E-2</v>
+      </c>
+      <c r="E31">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edited CRM accuracy calculation
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819E23B-AD51-4465-B4BA-7827ED93ADF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBD5F5-BC9A-ED4A-9F51-4EA2844F59D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="945" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11820" yWindow="500" windowWidth="16420" windowHeight="7880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -914,17 +914,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -944,7 +944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -965,7 +965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -986,7 +986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20210314</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20210314</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20210314</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20210314</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20210328</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20210328</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20210328</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20210328</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20210328</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20210404</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20210418</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20210428</v>
       </c>
@@ -1561,11 +1561,11 @@
         <v>2223.7829999999999</v>
       </c>
       <c r="C31">
-        <v>2225.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D31">
         <f t="shared" ref="D31" si="4">100*(B31-C31)/C31</f>
-        <v>-7.5804212143947045E-2</v>
+        <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
         <v>181</v>

</xml_diff>

<commit_message>
E5 initial test samples and blue tank titrations 0504 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819E23B-AD51-4465-B4BA-7827ED93ADF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B83C0CE-E48B-46CE-894D-903546DCEC43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="945" windowWidth="16425" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,16 +1561,37 @@
         <v>2223.7829999999999</v>
       </c>
       <c r="C31">
-        <v>2225.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31" si="4">100*(B31-C31)/C31</f>
-        <v>-7.5804212143947045E-2</v>
+        <f t="shared" ref="D31:D32" si="4">100*(B31-C31)/C31</f>
+        <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20210504</v>
+      </c>
+      <c r="B32">
+        <v>2224.8229999999999</v>
+      </c>
+      <c r="C32">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="4"/>
+        <v>1.5868948558535989E-2</v>
+      </c>
+      <c r="E32">
+        <v>180</v>
+      </c>
+      <c r="F32" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dmb ran blue tank titrations 0505
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B83C0CE-E48B-46CE-894D-903546DCEC43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A01D1B-C87A-4B7C-AB76-38710B09AE75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7710" yWindow="1455" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D32" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D33" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1592,6 +1592,27 @@
         <v>180</v>
       </c>
       <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20210505</v>
+      </c>
+      <c r="B33">
+        <v>2229.0880000000002</v>
+      </c>
+      <c r="C33">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="4"/>
+        <v>0.20760001258728566</v>
+      </c>
+      <c r="E33">
+        <v>180</v>
+      </c>
+      <c r="F33" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dmb ran more test samples for another run 0506
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A01D1B-C87A-4B7C-AB76-38710B09AE75}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5442D79-D0F0-4654-89F3-E045A5BA6FA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7710" yWindow="1455" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8490" yWindow="1005" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D33" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D34" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1613,6 +1613,27 @@
         <v>180</v>
       </c>
       <c r="F33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>20210506</v>
+      </c>
+      <c r="B34">
+        <v>2225.0940000000001</v>
+      </c>
+      <c r="C34">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="4"/>
+        <v>2.8051625780534287E-2</v>
+      </c>
+      <c r="E34">
+        <v>180</v>
+      </c>
+      <c r="F34" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dmb ran run5 samples for March 2020, ran first 9, 3 currently running
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5442D79-D0F0-4654-89F3-E045A5BA6FA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6A2093-7DCD-4F5B-A7F4-D9EF95861651}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="1005" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="1710" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D34" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D35" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1634,6 +1634,27 @@
         <v>180</v>
       </c>
       <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>20210511</v>
+      </c>
+      <c r="B35">
+        <v>2228.8789999999999</v>
+      </c>
+      <c r="C35">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>0.19820451613193732</v>
+      </c>
+      <c r="E35">
+        <v>180</v>
+      </c>
+      <c r="F35" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran rest of March TP2 run 1 samples and last sample from run5
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6A2093-7DCD-4F5B-A7F4-D9EF95861651}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA35B9D-B945-4EFE-A00D-2DF1BAD81896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1710" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="1020" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D35" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D36" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1655,6 +1655,27 @@
         <v>180</v>
       </c>
       <c r="F35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20210525</v>
+      </c>
+      <c r="B36">
+        <v>2223.5051632014602</v>
+      </c>
+      <c r="C36">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="4"/>
+        <v>-4.337378335242266E-2</v>
+      </c>
+      <c r="E36">
+        <v>180</v>
+      </c>
+      <c r="F36" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran three blue tank samples and rest of run 2 samples with one sample from run 3 for TP2 E5
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA35B9D-B945-4EFE-A00D-2DF1BAD81896}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137381E3-FFAC-40C4-9AD7-490DB019ACB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="1020" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="1710" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D36" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D37" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1676,6 +1676,27 @@
         <v>180</v>
       </c>
       <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20210526</v>
+      </c>
+      <c r="B37">
+        <v>2234.4699999999998</v>
+      </c>
+      <c r="C37">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="4"/>
+        <v>0.44954528494427892</v>
+      </c>
+      <c r="E37">
+        <v>180</v>
+      </c>
+      <c r="F37" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed rest of run 3 sampples for March 2020 TP2, processed 5 samples from run 4 for TP2
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137381E3-FFAC-40C4-9AD7-490DB019ACB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15DC0B5-8BF0-48E5-9CD0-2016A23BD32F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1365" yWindow="1710" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -912,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D37" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D38" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1684,19 +1684,40 @@
         <v>20210526</v>
       </c>
       <c r="B37">
-        <v>2234.4699999999998</v>
+        <v>2223.4699999999998</v>
       </c>
       <c r="C37">
         <v>2224.4699999999998</v>
       </c>
       <c r="D37">
         <f t="shared" si="4"/>
-        <v>0.44954528494427892</v>
+        <v>-4.4954528494427888E-2</v>
       </c>
       <c r="E37">
         <v>180</v>
       </c>
       <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>20210527</v>
+      </c>
+      <c r="B38">
+        <v>2221.3470000000002</v>
+      </c>
+      <c r="C38">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="4"/>
+        <v>-0.14039299248807999</v>
+      </c>
+      <c r="E38">
+        <v>180</v>
+      </c>
+      <c r="F38" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add titration data for TP2 run 6 and run 4 from 0601
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15DC0B5-8BF0-48E5-9CD0-2016A23BD32F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260B5FE3-5568-4BFF-88ED-439C228D3882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1710" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8250" yWindow="1065" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>CRM opened 20210418</t>
+  </si>
+  <si>
+    <t>CRM opened 20210526</t>
   </si>
 </sst>
 </file>
@@ -912,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1567,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D38" si="4">100*(B31-C31)/C31</f>
+        <f t="shared" ref="D31:D39" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
       <c r="E31">
@@ -1719,6 +1722,27 @@
       </c>
       <c r="F38" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>20210601</v>
+      </c>
+      <c r="B39">
+        <v>2222.2813428003801</v>
+      </c>
+      <c r="C39">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="4"/>
+        <v>-9.8390052444837811E-2</v>
+      </c>
+      <c r="E39">
+        <v>180</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weekly blue tank titrations, dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260B5FE3-5568-4BFF-88ED-439C228D3882}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BEC6F4-35FB-4453-88E4-DEEA6D770736}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8250" yWindow="1065" windowWidth="10200" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="1875" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -915,7 +915,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
@@ -1745,6 +1745,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>20210603</v>
+      </c>
+      <c r="B40">
+        <v>2228.9667413407301</v>
+      </c>
+      <c r="C40">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40" si="5">100*(B40-C40)/C40</f>
+        <v>0.20214888673393194</v>
+      </c>
+      <c r="E40">
+        <v>180</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added 0610 blue tank titrations, new temp probe
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BEC6F4-35FB-4453-88E4-DEEA6D770736}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9ADB3A-F6DF-4BEB-9E06-053F448AFBA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="1875" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6255" yWindow="1020" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>CRM opened 20210526</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20210526</t>
   </si>
 </sst>
 </file>
@@ -915,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,7 +1759,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D41" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1764,6 +1767,27 @@
       </c>
       <c r="F40" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>20210610</v>
+      </c>
+      <c r="B41">
+        <v>2229.3150000000001</v>
+      </c>
+      <c r="C41">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="5"/>
+        <v>0.21780469055551457</v>
+      </c>
+      <c r="E41">
+        <v>180</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weekly titrations for blue tanks dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9ADB3A-F6DF-4BEB-9E06-053F448AFBA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E8B21-6AC1-4A9E-A1B5-D552388AD55C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="1020" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9120" yWindow="30" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1759,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D41" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D42" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1787,6 +1787,27 @@
         <v>180</v>
       </c>
       <c r="F41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>20210615</v>
+      </c>
+      <c r="B42">
+        <v>2228.7220000000002</v>
+      </c>
+      <c r="C42">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="5"/>
+        <v>0.19114665515832571</v>
+      </c>
+      <c r="E42">
+        <v>180</v>
+      </c>
+      <c r="F42" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran blue tank and e5 titrations: run 6 and run 7 completed for march 2020
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E8B21-6AC1-4A9E-A1B5-D552388AD55C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659D0DF0-4973-41B8-BF1A-BB4DABE995CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="30" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="570" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>CRM OPENED 20210526</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20210624</t>
   </si>
 </sst>
 </file>
@@ -918,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1762,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D42" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D43" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1809,6 +1812,27 @@
       </c>
       <c r="F42" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>20210624</v>
+      </c>
+      <c r="B43">
+        <v>2228.4520000000002</v>
+      </c>
+      <c r="C43">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="5"/>
+        <v>0.17900893246483099</v>
+      </c>
+      <c r="E43">
+        <v>180</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run 8 and run 9 E5 titrations and blue tank titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659D0DF0-4973-41B8-BF1A-BB4DABE995CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27221008-5845-4F10-98C3-0EA16E1CA27E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="570" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9120" yWindow="480" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>CRM OPENED 20210624</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20210706</t>
   </si>
 </sst>
 </file>
@@ -921,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,7 +1765,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D43" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D44" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1833,6 +1836,27 @@
       </c>
       <c r="F43" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>20210706</v>
+      </c>
+      <c r="B44">
+        <v>2230.0918634412801</v>
+      </c>
+      <c r="C44">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="5"/>
+        <v>0.25272822026281822</v>
+      </c>
+      <c r="E44">
+        <v>180</v>
+      </c>
+      <c r="F44" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added E5 run 9 sample data dmb 0708
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27221008-5845-4F10-98C3-0EA16E1CA27E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93F7B0E-8D2B-418B-A9B5-E3A6C03538C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9120" yWindow="480" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9465" yWindow="825" windowWidth="10080" windowHeight="9255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>CRM OPENED 20210526</t>
-  </si>
-  <si>
-    <t>CRM OPENED 20210624</t>
-  </si>
-  <si>
-    <t>CRM OPENED 20210706</t>
   </si>
 </sst>
 </file>
@@ -924,15 +918,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1765,7 +1760,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D44" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D45" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1835,7 +1830,7 @@
         <v>180</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1856,7 +1851,28 @@
         <v>180</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>20210708</v>
+      </c>
+      <c r="B45">
+        <v>2228.9570833859798</v>
+      </c>
+      <c r="C45">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="5"/>
+        <v>0.20171471793191126</v>
+      </c>
+      <c r="E45">
+        <v>180</v>
+      </c>
+      <c r="F45" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
run 9 and 10 TA for E5 samples dmb 0715
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93F7B0E-8D2B-418B-A9B5-E3A6C03538C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C06B3B-BAEB-4F16-803E-4153481B8EDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9465" yWindow="825" windowWidth="10080" windowHeight="9255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9465" yWindow="825" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -918,10 +918,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,7 +1760,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D45" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D46" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1872,6 +1872,27 @@
         <v>180</v>
       </c>
       <c r="F45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>20210715</v>
+      </c>
+      <c r="B46">
+        <v>2230.4602923572402</v>
+      </c>
+      <c r="C46">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="5"/>
+        <v>0.26929076846351618</v>
+      </c>
+      <c r="E46">
+        <v>180</v>
+      </c>
+      <c r="F46" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
11 E5 samples for march 2020 dmb
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C06B3B-BAEB-4F16-803E-4153481B8EDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FA6359-E076-48FA-AB73-11E71F252AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9465" yWindow="825" windowWidth="10080" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7095" yWindow="375" windowWidth="11265" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>CRM OPENED 20210526</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20210720</t>
   </si>
 </sst>
 </file>
@@ -918,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,7 +1763,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D46" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D47" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1894,6 +1897,27 @@
       </c>
       <c r="F46" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>20210811</v>
+      </c>
+      <c r="B47">
+        <v>2221.0572992288098</v>
+      </c>
+      <c r="C47">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="5"/>
+        <v>-0.15341635406141577</v>
+      </c>
+      <c r="E47">
+        <v>180</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kristen TA Training added blue tank titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FA6359-E076-48FA-AB73-11E71F252AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96151933-E445-400B-A593-FBEC60B9AE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="375" windowWidth="11265" windowHeight="8595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>CRM OPENED 20210720</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20210721</t>
   </si>
 </sst>
 </file>
@@ -921,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,6 +1923,27 @@
         <v>14</v>
       </c>
     </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>20211018</v>
+      </c>
+      <c r="B48">
+        <v>2221.73708567331</v>
+      </c>
+      <c r="C48">
+        <v>2225.4699999999998</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48" si="6">100*(B48-C48)/C48</f>
+        <v>-0.16773599853917384</v>
+      </c>
+      <c r="E48">
+        <v>181</v>
+      </c>
+      <c r="F48" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed March 2020 TP2 run 11 and 7 samples of run 12
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96151933-E445-400B-A593-FBEC60B9AE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F405AD-4F24-4ED8-8CB6-7746BAD25B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,16 +1931,37 @@
         <v>2221.73708567331</v>
       </c>
       <c r="C48">
-        <v>2225.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48" si="6">100*(B48-C48)/C48</f>
-        <v>-0.16773599853917384</v>
+        <f t="shared" ref="D48:D49" si="6">100*(B48-C48)/C48</f>
+        <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
         <v>181</v>
       </c>
       <c r="F48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>20211110</v>
+      </c>
+      <c r="B49">
+        <v>2220.49470192943</v>
+      </c>
+      <c r="C49">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="6"/>
+        <v>-0.17870765038727457</v>
+      </c>
+      <c r="E49">
+        <v>181</v>
+      </c>
+      <c r="F49" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran updated cbls blue tank and quarantine tank TA dmbp
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F405AD-4F24-4ED8-8CB6-7746BAD25B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82284103-F04A-48D3-A57E-685BCFE831B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="795" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -77,7 +77,7 @@
     <t>CRM OPENED 20210720</t>
   </si>
   <si>
-    <t>CRM OPENED 20210721</t>
+    <t>CRM OPENED 20220118</t>
   </si>
 </sst>
 </file>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,14 +1934,14 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D49" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D52" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1959,9 +1959,72 @@
         <v>-0.17870765038727457</v>
       </c>
       <c r="E49">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>20211117</v>
+      </c>
+      <c r="B50">
+        <v>2231.6860000000001</v>
+      </c>
+      <c r="C50">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="6"/>
+        <v>0.32439187761580734</v>
+      </c>
+      <c r="E50">
+        <v>180</v>
+      </c>
+      <c r="F50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>20211206</v>
+      </c>
+      <c r="B51">
+        <v>2228.1970000000001</v>
+      </c>
+      <c r="C51">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="6"/>
+        <v>0.16754552769874698</v>
+      </c>
+      <c r="E51">
+        <v>180</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>20220118</v>
+      </c>
+      <c r="B52">
+        <v>2203.6729999999998</v>
+      </c>
+      <c r="C52">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="6"/>
+        <v>-0.93491932909861797</v>
+      </c>
+      <c r="E52">
+        <v>180</v>
+      </c>
+      <c r="F52" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cbls wetlab tank titrations, header tank 12 pm smbp
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82284103-F04A-48D3-A57E-685BCFE831B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFC3D66-AD26-42EE-B8C3-F1925EB14FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7695" yWindow="795" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D52" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D53" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2025,6 +2025,27 @@
         <v>180</v>
       </c>
       <c r="F52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>20220127</v>
+      </c>
+      <c r="B53">
+        <v>2231.4175319214601</v>
+      </c>
+      <c r="C53">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="6"/>
+        <v>0.31232302172923299</v>
+      </c>
+      <c r="E53">
+        <v>180</v>
+      </c>
+      <c r="F53" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DMBP ran titrations for cbls wetlab for another 12pm timepoint
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFC3D66-AD26-42EE-B8C3-F1925EB14FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C64E14-EF27-4B90-9128-FD82B28C27D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7695" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D53" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D54" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2046,6 +2046,27 @@
         <v>180</v>
       </c>
       <c r="F53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>20220131</v>
+      </c>
+      <c r="B54">
+        <v>2232.37</v>
+      </c>
+      <c r="C54">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="6"/>
+        <v>0.35514077510598441</v>
+      </c>
+      <c r="E54">
+        <v>180</v>
+      </c>
+      <c r="F54" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Titrations for 12pm timepoint for blue tanks and header tank and QT
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C64E14-EF27-4B90-9128-FD82B28C27D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC5AFEC-3C4D-40E3-811E-14AD3BBD23F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D54" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D55" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2067,6 +2067,27 @@
         <v>180</v>
       </c>
       <c r="F54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>20220201</v>
+      </c>
+      <c r="B55">
+        <v>2228.2564673073002</v>
+      </c>
+      <c r="C55">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="6"/>
+        <v>0.17021885245925669</v>
+      </c>
+      <c r="E55">
+        <v>180</v>
+      </c>
+      <c r="F55" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cbls wetlab titrations 12 pm
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC5AFEC-3C4D-40E3-811E-14AD3BBD23F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065687C9-A03E-4F65-94E3-150DED9272BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D55" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D56" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2088,6 +2088,27 @@
         <v>180</v>
       </c>
       <c r="F55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>20220203</v>
+      </c>
+      <c r="B56">
+        <v>2226.15763917096</v>
+      </c>
+      <c r="C56">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="6"/>
+        <v>7.5867023199243433E-2</v>
+      </c>
+      <c r="E56">
+        <v>180</v>
+      </c>
+      <c r="F56" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kristen completed tank titrations 0208
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065687C9-A03E-4F65-94E3-150DED9272BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6D7786-58A1-455E-BC39-287FE476BCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D56" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D57" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2109,6 +2109,27 @@
         <v>180</v>
       </c>
       <c r="F56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>20220209</v>
+      </c>
+      <c r="B57">
+        <v>2228.5439999999999</v>
+      </c>
+      <c r="C57">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="6"/>
+        <v>0.18314474908630232</v>
+      </c>
+      <c r="E57">
+        <v>180</v>
+      </c>
+      <c r="F57" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20220210 pierrick TA on E5 TP2 samples
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6D7786-58A1-455E-BC39-287FE476BCFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ADE043-9F2B-4A06-A516-F4B5966B9053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7695" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6735" yWindow="555" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D57" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D58" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2130,6 +2130,27 @@
         <v>180</v>
       </c>
       <c r="F57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>20220210</v>
+      </c>
+      <c r="B58">
+        <v>2228.61</v>
+      </c>
+      <c r="C58">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="6"/>
+        <v>0.18611174796694618</v>
+      </c>
+      <c r="E58">
+        <v>180</v>
+      </c>
+      <c r="F58" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed tank titrations 0216
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ADE043-9F2B-4A06-A516-F4B5966B9053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA31C62-FE3C-46B9-9915-EC224CA1326B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="555" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D58" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D59" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2151,6 +2151,27 @@
         <v>180</v>
       </c>
       <c r="F58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>20220216</v>
+      </c>
+      <c r="B59">
+        <v>2227.6280000000002</v>
+      </c>
+      <c r="C59">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="6"/>
+        <v>0.14196640098541929</v>
+      </c>
+      <c r="E59">
+        <v>180</v>
+      </c>
+      <c r="F59" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed tank titrations 0224
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA31C62-FE3C-46B9-9915-EC224CA1326B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF95AE1-095B-487C-91A7-E20CB628E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -924,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1934,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D59" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D60" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2172,6 +2172,27 @@
         <v>180</v>
       </c>
       <c r="F59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>20220224</v>
+      </c>
+      <c r="B60">
+        <v>2222.0050000000001</v>
+      </c>
+      <c r="C60">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="6"/>
+        <v>-0.11081291273875085</v>
+      </c>
+      <c r="E60">
+        <v>180</v>
+      </c>
+      <c r="F60" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed tank titrations 0302
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF95AE1-095B-487C-91A7-E20CB628E1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A5E15C-39AA-45BC-BA71-141A4046A3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="705" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220118</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220302</t>
   </si>
 </sst>
 </file>
@@ -924,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1937,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D60" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D61" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2194,6 +2197,27 @@
       </c>
       <c r="F60" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>20220302</v>
+      </c>
+      <c r="B61">
+        <v>2224.779</v>
+      </c>
+      <c r="C61">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="6"/>
+        <v>1.3890949304787049E-2</v>
+      </c>
+      <c r="E61">
+        <v>180</v>
+      </c>
+      <c r="F61" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed E5 titrations 0308
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8520016A-2075-489B-BA6D-8863389EDB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5511D89-21D0-452A-9D68-CEDC56887FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1305" windowWidth="11940" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1937,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D62" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D63" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2238,6 +2238,27 @@
         <v>180</v>
       </c>
       <c r="F62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>20220308</v>
+      </c>
+      <c r="B63">
+        <v>2220.8926944598902</v>
+      </c>
+      <c r="C63">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="6"/>
+        <v>-0.16081608383613138</v>
+      </c>
+      <c r="E63">
+        <v>180</v>
+      </c>
+      <c r="F63" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed bluetank titrations 0309
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5511D89-21D0-452A-9D68-CEDC56887FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53264B2F-3CB1-472C-86CD-09A924D49308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1937,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D63" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D64" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2259,6 +2259,27 @@
         <v>180</v>
       </c>
       <c r="F63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>20220309</v>
+      </c>
+      <c r="B64">
+        <v>2217.547</v>
+      </c>
+      <c r="C64">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="6"/>
+        <v>-0.31122020076691415</v>
+      </c>
+      <c r="E64">
+        <v>180</v>
+      </c>
+      <c r="F64" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0310 titrations and sample ID notation changes
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53264B2F-3CB1-472C-86CD-09A924D49308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B53317-D83C-4C63-B6C3-B1445B26C872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1937,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D64" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D65" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2280,6 +2280,27 @@
         <v>180</v>
       </c>
       <c r="F64" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>20220310</v>
+      </c>
+      <c r="B65">
+        <v>2221.9227812661102</v>
+      </c>
+      <c r="C65">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="6"/>
+        <v>-0.11450901715418155</v>
+      </c>
+      <c r="E65">
+        <v>180</v>
+      </c>
+      <c r="F65" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
export method and 20200314 titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B53317-D83C-4C63-B6C3-B1445B26C872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F299020-F3F8-41A5-8A62-B6FC1DE51AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -927,15 +927,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
@@ -1937,7 +1938,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D65" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D66" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2301,6 +2302,27 @@
         <v>180</v>
       </c>
       <c r="F65" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>20220314</v>
+      </c>
+      <c r="B66">
+        <v>2221.5278341974199</v>
+      </c>
+      <c r="C66">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="6"/>
+        <v>-0.13226367640740913</v>
+      </c>
+      <c r="E66">
+        <v>180</v>
+      </c>
+      <c r="F66" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20200317 samples, ph cal, CRM
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F299020-F3F8-41A5-8A62-B6FC1DE51AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6C689D-7EF7-4DC7-884E-8DA17C876EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220302</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220303</t>
   </si>
 </sst>
 </file>
@@ -927,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1941,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D66" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D68" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2324,6 +2327,48 @@
       </c>
       <c r="F66" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>20220315</v>
+      </c>
+      <c r="B67">
+        <v>2225.7539999999999</v>
+      </c>
+      <c r="C67">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="6"/>
+        <v>5.7721614586850156E-2</v>
+      </c>
+      <c r="E67">
+        <v>180</v>
+      </c>
+      <c r="F67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>20200317</v>
+      </c>
+      <c r="B68">
+        <v>2223.0121947257499</v>
+      </c>
+      <c r="C68">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="6"/>
+        <v>-6.5534948740596621E-2</v>
+      </c>
+      <c r="E68">
+        <v>180</v>
+      </c>
+      <c r="F68" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
friday monday titrations; pH cal; accuracy data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6C689D-7EF7-4DC7-884E-8DA17C876EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233BEB7-6961-4241-9A33-CAD7E10A5A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220303</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220318</t>
   </si>
 </sst>
 </file>
@@ -930,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1944,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D68" si="6">100*(B48-C48)/C48</f>
+        <f t="shared" ref="D48:D69" si="6">100*(B48-C48)/C48</f>
         <v>-0.12285687497200466</v>
       </c>
       <c r="E48">
@@ -2352,7 +2355,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>20200317</v>
+        <v>20220317</v>
       </c>
       <c r="B68">
         <v>2223.0121947257499</v>
@@ -2369,6 +2372,48 @@
       </c>
       <c r="F68" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>20220318</v>
+      </c>
+      <c r="B69">
+        <v>2226.3488441921399</v>
+      </c>
+      <c r="C69">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="6"/>
+        <v>8.4462554772154724E-2</v>
+      </c>
+      <c r="E69">
+        <v>180</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>20220321</v>
+      </c>
+      <c r="B70">
+        <v>2224.7499947312399</v>
+      </c>
+      <c r="C70">
+        <v>2225.4699999999998</v>
+      </c>
+      <c r="D70">
+        <f>100*(B70-C70)/C70</f>
+        <v>-3.2352953253016466E-2</v>
+      </c>
+      <c r="E70">
+        <v>180</v>
+      </c>
+      <c r="F70" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tuesday titrations 4 runs
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E233BEB7-6961-4241-9A33-CAD7E10A5A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEEF84E-18C0-4CD7-8EAA-3B291F24C46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1305" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -933,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2403,16 +2403,37 @@
         <v>2224.7499947312399</v>
       </c>
       <c r="C70">
-        <v>2225.4699999999998</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D70">
         <f>100*(B70-C70)/C70</f>
-        <v>-3.2352953253016466E-2</v>
+        <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
         <v>180</v>
       </c>
       <c r="F70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>20220322</v>
+      </c>
+      <c r="B71">
+        <v>2223.1790210232102</v>
+      </c>
+      <c r="C71">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D71">
+        <f>100*(B71-C71)/C71</f>
+        <v>-5.8035351197794287E-2</v>
+      </c>
+      <c r="E71">
+        <v>180</v>
+      </c>
+      <c r="F71" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
wednesday titrations for blue tank and E5
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEEF84E-18C0-4CD7-8EAA-3B291F24C46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EED83D-FF5E-4DF0-A312-9B16F32D797B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1305" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="705" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -933,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,6 +2437,27 @@
         <v>18</v>
       </c>
     </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>20220323</v>
+      </c>
+      <c r="B72">
+        <v>2227.4597991999999</v>
+      </c>
+      <c r="C72">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D72">
+        <f>100*(B72-C72)/C72</f>
+        <v>0.13440501332902252</v>
+      </c>
+      <c r="E72">
+        <v>180</v>
+      </c>
+      <c r="F72" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed E5 titrations 0329
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EED83D-FF5E-4DF0-A312-9B16F32D797B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7A2900-BBF4-4AA0-820B-12D06E857B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="705" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="705" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -933,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,6 +2458,27 @@
         <v>18</v>
       </c>
     </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>20220329</v>
+      </c>
+      <c r="B73">
+        <v>2234.105</v>
+      </c>
+      <c r="C73">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D73">
+        <f>100*(B73-C73)/C73</f>
+        <v>0.43313688204382256</v>
+      </c>
+      <c r="E73">
+        <v>180</v>
+      </c>
+      <c r="F73" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed tank titrations 0330
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7A2900-BBF4-4AA0-820B-12D06E857B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C892E6C-0124-4988-98C5-5AC6A6B32143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="705" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="645" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -933,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2479,6 +2479,27 @@
         <v>18</v>
       </c>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>20220330</v>
+      </c>
+      <c r="B74">
+        <v>2227.7080000000001</v>
+      </c>
+      <c r="C74">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D74">
+        <f>100*(B74-C74)/C74</f>
+        <v>0.14556276326497025</v>
+      </c>
+      <c r="E74">
+        <v>180</v>
+      </c>
+      <c r="F74" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed E5 titrations 0331
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C892E6C-0124-4988-98C5-5AC6A6B32143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212848E3-F785-4060-922D-2350A8F0587A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="645" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="975" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -933,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,6 +2500,27 @@
         <v>18</v>
       </c>
     </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>20220331</v>
+      </c>
+      <c r="B75">
+        <v>2226.165</v>
+      </c>
+      <c r="C75">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D75">
+        <f>100*(B75-C75)/C75</f>
+        <v>7.619792579806263E-2</v>
+      </c>
+      <c r="E75">
+        <v>180</v>
+      </c>
+      <c r="F75" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
last week of titration data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212848E3-F785-4060-922D-2350A8F0587A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98B0079-38A4-4166-A75C-8989F558F2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="975" windowWidth="14535" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220318</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220401 MG</t>
   </si>
 </sst>
 </file>
@@ -933,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,7 +2409,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D70">
-        <f>100*(B70-C70)/C70</f>
+        <f t="shared" ref="D70:D77" si="7">100*(B70-C70)/C70</f>
         <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
@@ -2427,7 +2430,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D71">
-        <f>100*(B71-C71)/C71</f>
+        <f t="shared" si="7"/>
         <v>-5.8035351197794287E-2</v>
       </c>
       <c r="E71">
@@ -2448,7 +2451,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D72">
-        <f>100*(B72-C72)/C72</f>
+        <f t="shared" si="7"/>
         <v>0.13440501332902252</v>
       </c>
       <c r="E72">
@@ -2469,7 +2472,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D73">
-        <f>100*(B73-C73)/C73</f>
+        <f t="shared" si="7"/>
         <v>0.43313688204382256</v>
       </c>
       <c r="E73">
@@ -2490,7 +2493,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D74">
-        <f>100*(B74-C74)/C74</f>
+        <f t="shared" si="7"/>
         <v>0.14556276326497025</v>
       </c>
       <c r="E74">
@@ -2511,7 +2514,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D75">
-        <f>100*(B75-C75)/C75</f>
+        <f t="shared" si="7"/>
         <v>7.619792579806263E-2</v>
       </c>
       <c r="E75">
@@ -2519,6 +2522,48 @@
       </c>
       <c r="F75" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>20220401</v>
+      </c>
+      <c r="B76">
+        <v>2225.92</v>
+      </c>
+      <c r="C76">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="7"/>
+        <v>6.5184066316932701E-2</v>
+      </c>
+      <c r="E76">
+        <v>180</v>
+      </c>
+      <c r="F76" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>20220404</v>
+      </c>
+      <c r="B77">
+        <v>2224.5797358742998</v>
+      </c>
+      <c r="C77">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="7"/>
+        <v>4.9331244880796727E-3</v>
+      </c>
+      <c r="E77">
+        <v>180</v>
+      </c>
+      <c r="F77" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed tank titrations 0413
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0879AD89-B51C-477A-B714-22F118CA7872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FF9C7A-AEC9-4970-B319-FF21DE8E4264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6270" yWindow="615" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -936,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2409,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D80" si="7">100*(B70-C70)/C70</f>
+        <f t="shared" ref="D70:D81" si="7">100*(B70-C70)/C70</f>
         <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
@@ -2626,6 +2626,27 @@
         <v>180</v>
       </c>
       <c r="F80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>20220413</v>
+      </c>
+      <c r="B81">
+        <v>2223.6496216999999</v>
+      </c>
+      <c r="C81">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="7"/>
+        <v>-3.687971966355591E-2</v>
+      </c>
+      <c r="E81">
+        <v>180</v>
+      </c>
+      <c r="F81" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed tank titrations 0420
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FF9C7A-AEC9-4970-B319-FF21DE8E4264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB93B55-4EE7-4D06-A450-62C9B827E5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="615" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -936,10 +936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F81"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2409,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D81" si="7">100*(B70-C70)/C70</f>
+        <f t="shared" ref="D70:D82" si="7">100*(B70-C70)/C70</f>
         <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
@@ -2647,6 +2647,27 @@
         <v>180</v>
       </c>
       <c r="F81" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>20220420</v>
+      </c>
+      <c r="B82">
+        <v>2225.2184000000002</v>
+      </c>
+      <c r="C82">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="7"/>
+        <v>3.3643969125247891E-2</v>
+      </c>
+      <c r="E82">
+        <v>180</v>
+      </c>
+      <c r="F82" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed tank titrations 0427
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB93B55-4EE7-4D06-A450-62C9B827E5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689342DD-C1B9-4F64-AFE0-904E36BBBE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6270" yWindow="615" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220401 MG</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220427</t>
   </si>
 </sst>
 </file>
@@ -936,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2412,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D82" si="7">100*(B70-C70)/C70</f>
+        <f t="shared" ref="D70:D83" si="7">100*(B70-C70)/C70</f>
         <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
@@ -2669,6 +2672,27 @@
       </c>
       <c r="F82" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>20220427</v>
+      </c>
+      <c r="B83">
+        <v>2215.5293579999998</v>
+      </c>
+      <c r="C83">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="7"/>
+        <v>-0.40192234554747991</v>
+      </c>
+      <c r="E83">
+        <v>180</v>
+      </c>
+      <c r="F83" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed tank titrations 0504
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689342DD-C1B9-4F64-AFE0-904E36BBBE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D674D6B1-0B86-4EFC-8535-670DF2614739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="615" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-240" yWindow="450" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -939,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2412,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D83" si="7">100*(B70-C70)/C70</f>
+        <f t="shared" ref="D70:D84" si="7">100*(B70-C70)/C70</f>
         <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
@@ -2692,6 +2692,27 @@
         <v>180</v>
       </c>
       <c r="F83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>20220504</v>
+      </c>
+      <c r="B84">
+        <v>2200.1692800000001</v>
+      </c>
+      <c r="C84">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="7"/>
+        <v>-1.0924274096751014</v>
+      </c>
+      <c r="E84">
+        <v>180</v>
+      </c>
+      <c r="F84" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran blue tank titratons 0518 dmbp
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D674D6B1-0B86-4EFC-8535-670DF2614739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE656D51-F861-4119-A98C-9263C722CE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="450" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="705" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220427</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220518</t>
   </si>
 </sst>
 </file>
@@ -939,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2415,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D84" si="7">100*(B70-C70)/C70</f>
+        <f t="shared" ref="D70:D85" si="7">100*(B70-C70)/C70</f>
         <v>1.258703112382251E-2</v>
       </c>
       <c r="E70">
@@ -2714,6 +2717,27 @@
       </c>
       <c r="F84" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>20220518</v>
+      </c>
+      <c r="B85">
+        <v>2201.1546499999999</v>
+      </c>
+      <c r="C85">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="7"/>
+        <v>-1.0481305659325526</v>
+      </c>
+      <c r="E85">
+        <v>180</v>
+      </c>
+      <c r="F85" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
titrator training dmbp and lz, changed new acid titrant bottle, blue tank titrations dmbp 0608
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE656D51-F861-4119-A98C-9263C722CE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FC8615-2C4E-4360-952D-48FA9958C347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="705" windowWidth="10260" windowHeight="10215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="765" windowWidth="11625" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220518</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220427 dmbp</t>
   </si>
 </sst>
 </file>
@@ -942,15 +945,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
@@ -2740,6 +2743,27 @@
         <v>21</v>
       </c>
     </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>20220608</v>
+      </c>
+      <c r="B86">
+        <v>2228.8510392501998</v>
+      </c>
+      <c r="C86">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D86">
+        <f t="shared" ref="D86" si="8">100*(B86-C86)/C86</f>
+        <v>0.19694755380832502</v>
+      </c>
+      <c r="E86">
+        <v>180</v>
+      </c>
+      <c r="F86" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LZ titrations; updated CBLS aquarium script
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65FC8615-2C4E-4360-952D-48FA9958C347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B89942-B8FF-41C4-848E-BD895FE27987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="765" windowWidth="11625" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15255" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -100,12 +100,15 @@
   <si>
     <t>CRM OPENED 20220427 dmbp</t>
   </si>
+  <si>
+    <t>CRM OPENED 20220427 DMBP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +248,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -588,8 +597,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -945,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,7 +2766,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D86">
-        <f t="shared" ref="D86" si="8">100*(B86-C86)/C86</f>
+        <f>100*(B86-C86)/C86</f>
         <v>0.19694755380832502</v>
       </c>
       <c r="E86">
@@ -2762,6 +2774,27 @@
       </c>
       <c r="F86" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>20220720</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2208.6642099999999</v>
+      </c>
+      <c r="C87">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D87">
+        <f>100*(B87-C87)/C87</f>
+        <v>-0.7105418369319384</v>
+      </c>
+      <c r="E87">
+        <v>180</v>
+      </c>
+      <c r="F87" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LZ E5 and CBLS titrations 20220729
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC5B3CD-72BE-43A3-A59F-B7CDF753D794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E49DBCF-7428-4EC3-A67A-886C62E03FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="165" windowWidth="15255" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="765" windowWidth="10290" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>CRM OPENED AND TESTED 20220722 LHZ</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220722 LHZ</t>
   </si>
 </sst>
 </file>
@@ -963,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F91"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,14 +2880,35 @@
         <v>2226.38</v>
       </c>
       <c r="D91">
-        <f t="shared" si="8"/>
-        <v>-1.1512880550490059</v>
+        <f>D92</f>
+        <v>7.1615261163340063E-2</v>
       </c>
       <c r="E91">
         <v>176</v>
       </c>
       <c r="F91" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>20220729</v>
+      </c>
+      <c r="B92">
+        <v>2226.06306</v>
+      </c>
+      <c r="C92">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D92">
+        <f>100*(B92-C92)/C92</f>
+        <v>7.1615261163340063E-2</v>
+      </c>
+      <c r="E92">
+        <v>180</v>
+      </c>
+      <c r="F92" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LZ BT titrations 20220802
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E49DBCF-7428-4EC3-A67A-886C62E03FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE15308-24D3-4ACD-846F-298A5EF2CC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="765" windowWidth="10290" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220722 LHZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRM OPENED 20220702 </t>
   </si>
 </sst>
 </file>
@@ -966,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,7 +2862,7 @@
         <v>2226.38</v>
       </c>
       <c r="D90">
-        <f t="shared" ref="D90:D91" si="8">100*(B90-C90)/C90</f>
+        <f t="shared" ref="D90" si="8">100*(B90-C90)/C90</f>
         <v>-0.49911039445198346</v>
       </c>
       <c r="E90">
@@ -2909,6 +2912,27 @@
       </c>
       <c r="F92" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>20220802</v>
+      </c>
+      <c r="B93">
+        <v>2220.3086600000001</v>
+      </c>
+      <c r="C93">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D93">
+        <f>100*(B93-C93)/C93</f>
+        <v>-0.18707107760498703</v>
+      </c>
+      <c r="E93">
+        <v>180</v>
+      </c>
+      <c r="F93" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LZ 20220831 BT titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17758EB3-65FB-4D6D-AC91-1EC53739F0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054A8078-1072-4815-AEFF-CB5E88260BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -979,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,6 +2966,27 @@
         <v>28</v>
       </c>
     </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>20220831</v>
+      </c>
+      <c r="B95">
+        <v>2210.5472799999998</v>
+      </c>
+      <c r="C95">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D95">
+        <f>100*(B95-C95)/C95</f>
+        <v>-0.62588931295994232</v>
+      </c>
+      <c r="E95">
+        <v>180</v>
+      </c>
+      <c r="F95" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LZ BT Titrations 20230209
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054A8078-1072-4815-AEFF-CB5E88260BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C65B2F-FF2D-44E9-94EA-5C3B8A0AAD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14490" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,42 @@
   </si>
   <si>
     <t>CRM OPENED 20220825 LHZ</t>
+  </si>
+  <si>
+    <t>pH probe may have dried out, leading to a misleading value here…trying again tomorrow</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220722</t>
+  </si>
+  <si>
+    <t>176 (TestB)</t>
+  </si>
+  <si>
+    <t>176 (TestA)</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220722 (TA calculated based on pHCalibration from 0916)</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220930 (TA calculated based on pH calibration 0916)</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20210719</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220401</t>
+  </si>
+  <si>
+    <t>CRMUNLABELEDOPENINGDATE</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220930</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20230118</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20220908 (Don't recommend using this Batch bottle)</t>
   </si>
 </sst>
 </file>
@@ -618,12 +654,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -979,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,7 +1859,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:D47" si="5">100*(B40-C40)/C40</f>
+        <f t="shared" ref="D40:D51" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
       <c r="E40">
@@ -1960,1031 +1997,1556 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>20210811</v>
+        <v>20210719</v>
       </c>
       <c r="B47">
-        <v>2221.0572992288098</v>
+        <v>2226.4870498855298</v>
       </c>
       <c r="C47">
         <v>2224.4699999999998</v>
       </c>
       <c r="D47">
         <f t="shared" si="5"/>
-        <v>-0.15341635406141577</v>
+        <v>9.0675526553741517E-2</v>
       </c>
       <c r="E47">
         <v>180</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>20211018</v>
+        <v>20210723</v>
       </c>
       <c r="B48">
-        <v>2221.73708567331</v>
+        <v>2231.0569999999998</v>
       </c>
       <c r="C48">
         <v>2224.4699999999998</v>
       </c>
       <c r="D48">
-        <f t="shared" ref="D48:D69" si="6">100*(B48-C48)/C48</f>
-        <v>-0.12285687497200466</v>
+        <f t="shared" si="5"/>
+        <v>0.29611547919279602</v>
       </c>
       <c r="E48">
         <v>180</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
+        <v>20210724</v>
+      </c>
+      <c r="B49">
+        <v>2227.3916066216202</v>
+      </c>
+      <c r="C49">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="5"/>
+        <v>0.13133944812114404</v>
+      </c>
+      <c r="E49">
+        <v>180</v>
+      </c>
+      <c r="F49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>20210730</v>
+      </c>
+      <c r="B50">
+        <v>2225.6402336351998</v>
+      </c>
+      <c r="C50">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="5"/>
+        <v>5.2607301298737238E-2</v>
+      </c>
+      <c r="E50">
+        <v>180</v>
+      </c>
+      <c r="F50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>20210811</v>
+      </c>
+      <c r="B51">
+        <v>2221.0572992288098</v>
+      </c>
+      <c r="C51">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="5"/>
+        <v>-0.15341635406141577</v>
+      </c>
+      <c r="E51">
+        <v>180</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>20211018</v>
+      </c>
+      <c r="B52">
+        <v>2221.73708567331</v>
+      </c>
+      <c r="C52">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ref="D52:D74" si="6">100*(B52-C52)/C52</f>
+        <v>-0.12285687497200466</v>
+      </c>
+      <c r="E52">
+        <v>180</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>20211110</v>
       </c>
-      <c r="B49">
+      <c r="B53">
         <v>2220.49470192943</v>
       </c>
-      <c r="C49">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D49">
+      <c r="C53">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D53">
         <f t="shared" si="6"/>
         <v>-0.17870765038727457</v>
       </c>
-      <c r="E49">
-        <v>180</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E53">
+        <v>180</v>
+      </c>
+      <c r="F53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>20211117</v>
       </c>
-      <c r="B50">
+      <c r="B54">
         <v>2231.6860000000001</v>
       </c>
-      <c r="C50">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D50">
+      <c r="C54">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D54">
         <f t="shared" si="6"/>
         <v>0.32439187761580734</v>
       </c>
-      <c r="E50">
-        <v>180</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E54">
+        <v>180</v>
+      </c>
+      <c r="F54" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>20211206</v>
       </c>
-      <c r="B51">
+      <c r="B55">
         <v>2228.1970000000001</v>
       </c>
-      <c r="C51">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D51">
+      <c r="C55">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D55">
         <f t="shared" si="6"/>
         <v>0.16754552769874698</v>
       </c>
-      <c r="E51">
-        <v>180</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E55">
+        <v>180</v>
+      </c>
+      <c r="F55" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>20220118</v>
       </c>
-      <c r="B52">
+      <c r="B56">
         <v>2203.6729999999998</v>
       </c>
-      <c r="C52">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D52">
+      <c r="C56">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D56">
         <f t="shared" si="6"/>
         <v>-0.93491932909861797</v>
       </c>
-      <c r="E52">
-        <v>180</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E56">
+        <v>180</v>
+      </c>
+      <c r="F56" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>20220127</v>
       </c>
-      <c r="B53">
+      <c r="B57">
         <v>2231.4175319214601</v>
       </c>
-      <c r="C53">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D53">
+      <c r="C57">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D57">
         <f t="shared" si="6"/>
         <v>0.31232302172923299</v>
       </c>
-      <c r="E53">
-        <v>180</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E57">
+        <v>180</v>
+      </c>
+      <c r="F57" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>20220131</v>
       </c>
-      <c r="B54">
+      <c r="B58">
         <v>2232.37</v>
       </c>
-      <c r="C54">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D54">
+      <c r="C58">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D58">
         <f t="shared" si="6"/>
         <v>0.35514077510598441</v>
       </c>
-      <c r="E54">
-        <v>180</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="E58">
+        <v>180</v>
+      </c>
+      <c r="F58" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>20220201</v>
       </c>
-      <c r="B55">
+      <c r="B59">
         <v>2228.2564673073002</v>
       </c>
-      <c r="C55">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D55">
+      <c r="C59">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D59">
         <f t="shared" si="6"/>
         <v>0.17021885245925669</v>
       </c>
-      <c r="E55">
-        <v>180</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E59">
+        <v>180</v>
+      </c>
+      <c r="F59" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>20220203</v>
       </c>
-      <c r="B56">
+      <c r="B60">
         <v>2226.15763917096</v>
       </c>
-      <c r="C56">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D56">
+      <c r="C60">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="6"/>
         <v>7.5867023199243433E-2</v>
       </c>
-      <c r="E56">
-        <v>180</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E60">
+        <v>180</v>
+      </c>
+      <c r="F60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>20220209</v>
       </c>
-      <c r="B57">
+      <c r="B61">
         <v>2228.5439999999999</v>
       </c>
-      <c r="C57">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D57">
+      <c r="C61">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="6"/>
         <v>0.18314474908630232</v>
       </c>
-      <c r="E57">
-        <v>180</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E61">
+        <v>180</v>
+      </c>
+      <c r="F61" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>20220210</v>
       </c>
-      <c r="B58">
+      <c r="B62">
         <v>2228.61</v>
       </c>
-      <c r="C58">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D58">
+      <c r="C62">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D62">
         <f t="shared" si="6"/>
         <v>0.18611174796694618</v>
       </c>
-      <c r="E58">
-        <v>180</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E62">
+        <v>180</v>
+      </c>
+      <c r="F62" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>20220216</v>
       </c>
-      <c r="B59">
+      <c r="B63">
         <v>2227.6280000000002</v>
       </c>
-      <c r="C59">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D59">
+      <c r="C63">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D63">
         <f t="shared" si="6"/>
         <v>0.14196640098541929</v>
       </c>
-      <c r="E59">
-        <v>180</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E63">
+        <v>180</v>
+      </c>
+      <c r="F63" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>20220224</v>
       </c>
-      <c r="B60">
+      <c r="B64">
         <v>2222.0050000000001</v>
       </c>
-      <c r="C60">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D60">
+      <c r="C64">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D64">
         <f t="shared" si="6"/>
         <v>-0.11081291273875085</v>
       </c>
-      <c r="E60">
-        <v>180</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E64">
+        <v>180</v>
+      </c>
+      <c r="F64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>20220302</v>
       </c>
-      <c r="B61">
+      <c r="B65">
         <v>2224.779</v>
       </c>
-      <c r="C61">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D61">
+      <c r="C65">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D65">
         <f t="shared" si="6"/>
         <v>1.3890949304787049E-2</v>
       </c>
-      <c r="E61">
-        <v>180</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E65">
+        <v>180</v>
+      </c>
+      <c r="F65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>20220303</v>
       </c>
-      <c r="B62">
+      <c r="B66">
         <v>2221.846</v>
       </c>
-      <c r="C62">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D62">
+      <c r="C66">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D66">
         <f t="shared" si="6"/>
         <v>-0.11796068276936962</v>
       </c>
-      <c r="E62">
-        <v>180</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E66">
+        <v>180</v>
+      </c>
+      <c r="F66" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>20220308</v>
       </c>
-      <c r="B63">
+      <c r="B67">
         <v>2220.8926944598902</v>
       </c>
-      <c r="C63">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D63">
+      <c r="C67">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="6"/>
         <v>-0.16081608383613138</v>
       </c>
-      <c r="E63">
-        <v>180</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E67">
+        <v>180</v>
+      </c>
+      <c r="F67" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>20220309</v>
       </c>
-      <c r="B64">
+      <c r="B68">
         <v>2217.547</v>
       </c>
-      <c r="C64">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D64">
+      <c r="C68">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="6"/>
         <v>-0.31122020076691415</v>
       </c>
-      <c r="E64">
-        <v>180</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E68">
+        <v>180</v>
+      </c>
+      <c r="F68" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
         <v>20220310</v>
       </c>
-      <c r="B65">
+      <c r="B69">
         <v>2221.9227812661102</v>
       </c>
-      <c r="C65">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D65">
+      <c r="C69">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="6"/>
         <v>-0.11450901715418155</v>
       </c>
-      <c r="E65">
-        <v>180</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E69">
+        <v>180</v>
+      </c>
+      <c r="F69" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>20220311</v>
+      </c>
+      <c r="B70">
+        <v>2226.5838482945901</v>
+      </c>
+      <c r="C70">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="6"/>
+        <v>9.5027053392057345E-2</v>
+      </c>
+      <c r="E70">
+        <v>180</v>
+      </c>
+      <c r="F70" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>20220314</v>
       </c>
-      <c r="B66">
+      <c r="B71">
         <v>2221.5278341974199</v>
       </c>
-      <c r="C66">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D66">
+      <c r="C71">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D71">
         <f t="shared" si="6"/>
         <v>-0.13226367640740913</v>
       </c>
-      <c r="E66">
-        <v>180</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E71">
+        <v>180</v>
+      </c>
+      <c r="F71" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>20220315</v>
       </c>
-      <c r="B67">
+      <c r="B72">
         <v>2225.7539999999999</v>
       </c>
-      <c r="C67">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D67">
+      <c r="C72">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D72">
         <f t="shared" si="6"/>
         <v>5.7721614586850156E-2</v>
       </c>
-      <c r="E67">
-        <v>180</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E72">
+        <v>180</v>
+      </c>
+      <c r="F72" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>20220317</v>
       </c>
-      <c r="B68">
+      <c r="B73">
         <v>2223.0121947257499</v>
       </c>
-      <c r="C68">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D68">
+      <c r="C73">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D73">
         <f t="shared" si="6"/>
         <v>-6.5534948740596621E-2</v>
       </c>
-      <c r="E68">
-        <v>180</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E73">
+        <v>180</v>
+      </c>
+      <c r="F73" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>20220318</v>
       </c>
-      <c r="B69">
+      <c r="B74">
         <v>2226.3488441921399</v>
       </c>
-      <c r="C69">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D69">
+      <c r="C74">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D74">
         <f t="shared" si="6"/>
         <v>8.4462554772154724E-2</v>
       </c>
-      <c r="E69">
-        <v>180</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E74">
+        <v>180</v>
+      </c>
+      <c r="F74" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>20220321</v>
       </c>
-      <c r="B70">
+      <c r="B75">
         <v>2224.7499947312399</v>
       </c>
-      <c r="C70">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D70">
-        <f t="shared" ref="D70:D85" si="7">100*(B70-C70)/C70</f>
+      <c r="C75">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:D94" si="7">100*(B75-C75)/C75</f>
         <v>1.258703112382251E-2</v>
       </c>
-      <c r="E70">
-        <v>180</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E75">
+        <v>180</v>
+      </c>
+      <c r="F75" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>20220322</v>
       </c>
-      <c r="B71">
+      <c r="B76">
         <v>2223.1790210232102</v>
       </c>
-      <c r="C71">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D71">
+      <c r="C76">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D76">
         <f t="shared" si="7"/>
         <v>-5.8035351197794287E-2</v>
       </c>
-      <c r="E71">
-        <v>180</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E76">
+        <v>180</v>
+      </c>
+      <c r="F76" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>20220323</v>
       </c>
-      <c r="B72">
+      <c r="B77">
         <v>2227.4597991999999</v>
       </c>
-      <c r="C72">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D72">
+      <c r="C77">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="7"/>
         <v>0.13440501332902252</v>
       </c>
-      <c r="E72">
-        <v>180</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E77">
+        <v>180</v>
+      </c>
+      <c r="F77" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>20220324</v>
+      </c>
+      <c r="B78">
+        <v>2220.70646995792</v>
+      </c>
+      <c r="C78">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="7"/>
+        <v>-0.16918771851631018</v>
+      </c>
+      <c r="E78">
+        <v>180</v>
+      </c>
+      <c r="F78" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>20220329</v>
       </c>
-      <c r="B73">
+      <c r="B79">
         <v>2234.105</v>
       </c>
-      <c r="C73">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D73">
+      <c r="C79">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="7"/>
         <v>0.43313688204382256</v>
       </c>
-      <c r="E73">
-        <v>180</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="E79">
+        <v>180</v>
+      </c>
+      <c r="F79" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>20220330</v>
       </c>
-      <c r="B74">
+      <c r="B80">
         <v>2227.7080000000001</v>
       </c>
-      <c r="C74">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D74">
+      <c r="C80">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D80">
         <f t="shared" si="7"/>
         <v>0.14556276326497025</v>
       </c>
-      <c r="E74">
-        <v>180</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E80">
+        <v>180</v>
+      </c>
+      <c r="F80" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
         <v>20220331</v>
       </c>
-      <c r="B75">
+      <c r="B81">
         <v>2226.165</v>
       </c>
-      <c r="C75">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D75">
+      <c r="C81">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D81">
         <f t="shared" si="7"/>
         <v>7.619792579806263E-2</v>
       </c>
-      <c r="E75">
-        <v>180</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="E81">
+        <v>180</v>
+      </c>
+      <c r="F81" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
         <v>20220401</v>
       </c>
-      <c r="B76">
+      <c r="B82">
         <v>2225.92</v>
       </c>
-      <c r="C76">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D76">
+      <c r="C82">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D82">
         <f t="shared" si="7"/>
         <v>6.5184066316932701E-2</v>
       </c>
-      <c r="E76">
-        <v>180</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="E82">
+        <v>180</v>
+      </c>
+      <c r="F82" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>20220404</v>
       </c>
-      <c r="B77">
+      <c r="B83">
         <v>2224.5797358742998</v>
       </c>
-      <c r="C77">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D77">
+      <c r="C83">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D83">
         <f t="shared" si="7"/>
         <v>4.9331244880796727E-3</v>
       </c>
-      <c r="E77">
-        <v>180</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="E83">
+        <v>180</v>
+      </c>
+      <c r="F83" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
         <v>20220405</v>
       </c>
-      <c r="B78">
+      <c r="B84">
         <v>2221.9426290986098</v>
       </c>
-      <c r="C78">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D78">
+      <c r="C84">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D84">
         <f t="shared" si="7"/>
         <v>-0.11361676720252403</v>
       </c>
-      <c r="E78">
-        <v>180</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="E84">
+        <v>180</v>
+      </c>
+      <c r="F84" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>20220406</v>
       </c>
-      <c r="B79">
+      <c r="B85">
         <v>2219.3566865192001</v>
       </c>
-      <c r="C79">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D79">
+      <c r="C85">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D85">
         <f t="shared" si="7"/>
         <v>-0.22986659657355063</v>
       </c>
-      <c r="E79">
-        <v>180</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="E85">
+        <v>180</v>
+      </c>
+      <c r="F85" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
         <v>20220407</v>
       </c>
-      <c r="B80">
+      <c r="B86">
         <v>2226.1503724982399</v>
       </c>
-      <c r="C80">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D80">
+      <c r="C86">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D86">
         <f t="shared" si="7"/>
         <v>7.5540353353387713E-2</v>
       </c>
-      <c r="E80">
-        <v>180</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E86">
+        <v>180</v>
+      </c>
+      <c r="F86" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>20220408</v>
+      </c>
+      <c r="B87">
+        <v>2220.60904733079</v>
+      </c>
+      <c r="C87">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="7"/>
+        <v>-0.17356730678363105</v>
+      </c>
+      <c r="E87">
+        <v>180</v>
+      </c>
+      <c r="F87" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
         <v>20220413</v>
       </c>
-      <c r="B81">
+      <c r="B88">
         <v>2223.6496216999999</v>
       </c>
-      <c r="C81">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D81">
+      <c r="C88">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D88">
         <f t="shared" si="7"/>
         <v>-3.687971966355591E-2</v>
       </c>
-      <c r="E81">
-        <v>180</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="E88">
+        <v>180</v>
+      </c>
+      <c r="F88" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>20220415</v>
+      </c>
+      <c r="B89">
+        <v>2223.5663069920402</v>
+      </c>
+      <c r="C89">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="7"/>
+        <v>-4.0625093076537153E-2</v>
+      </c>
+      <c r="E89">
+        <v>180</v>
+      </c>
+      <c r="F89" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>20220420</v>
       </c>
-      <c r="B82">
+      <c r="B90">
         <v>2225.2184000000002</v>
       </c>
-      <c r="C82">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D82">
+      <c r="C90">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D90">
         <f t="shared" si="7"/>
         <v>3.3643969125247891E-2</v>
       </c>
-      <c r="E82">
-        <v>180</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E90">
+        <v>180</v>
+      </c>
+      <c r="F90" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
         <v>20220427</v>
       </c>
-      <c r="B83">
+      <c r="B91">
         <v>2215.5293579999998</v>
       </c>
-      <c r="C83">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D83">
+      <c r="C91">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D91">
         <f t="shared" si="7"/>
         <v>-0.40192234554747991</v>
       </c>
-      <c r="E83">
-        <v>180</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E91">
+        <v>180</v>
+      </c>
+      <c r="F91" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
         <v>20220504</v>
       </c>
-      <c r="B84">
+      <c r="B92">
         <v>2200.1692800000001</v>
       </c>
-      <c r="C84">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D84">
+      <c r="C92">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D92">
         <f t="shared" si="7"/>
         <v>-1.0924274096751014</v>
       </c>
-      <c r="E84">
-        <v>180</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E92">
+        <v>180</v>
+      </c>
+      <c r="F92" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>20220518</v>
       </c>
-      <c r="B85">
+      <c r="B93">
         <v>2201.1546499999999</v>
       </c>
-      <c r="C85">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D85">
+      <c r="C93">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D93">
         <f t="shared" si="7"/>
         <v>-1.0481305659325526</v>
       </c>
-      <c r="E85">
-        <v>180</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E93">
+        <v>180</v>
+      </c>
+      <c r="F93" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>20220608</v>
-      </c>
-      <c r="B86">
-        <v>2228.8510392501998</v>
-      </c>
-      <c r="C86">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D86">
-        <f>100*(B86-C86)/C86</f>
-        <v>0.19694755380832502</v>
-      </c>
-      <c r="E86">
-        <v>180</v>
-      </c>
-      <c r="F86" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>20220720</v>
-      </c>
-      <c r="B87" s="1">
-        <v>2208.6642099999999</v>
-      </c>
-      <c r="C87">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D87">
-        <f>100*(B87-C87)/C87</f>
-        <v>-0.7105418369319384</v>
-      </c>
-      <c r="E87">
-        <v>180</v>
-      </c>
-      <c r="F87" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>20220722</v>
-      </c>
-      <c r="B88" s="1">
-        <v>2217.8699700000002</v>
-      </c>
-      <c r="C88">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D88">
-        <f>100*(B88-C88)/C88</f>
-        <v>-0.29670123669906118</v>
-      </c>
-      <c r="E88">
-        <v>180</v>
-      </c>
-      <c r="F88" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>20220722</v>
-      </c>
-      <c r="B89">
-        <v>2217.323202</v>
-      </c>
-      <c r="C89">
-        <v>2226.38</v>
-      </c>
-      <c r="D89">
-        <f>100*(B89-C89)/C89</f>
-        <v>-0.40679479693493792</v>
-      </c>
-      <c r="E89">
-        <v>176</v>
-      </c>
-      <c r="F89" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>20220722</v>
-      </c>
-      <c r="B90">
-        <v>2215.267906</v>
-      </c>
-      <c r="C90">
-        <v>2226.38</v>
-      </c>
-      <c r="D90">
-        <f t="shared" ref="D90" si="8">100*(B90-C90)/C90</f>
-        <v>-0.49911039445198346</v>
-      </c>
-      <c r="E90">
-        <v>176</v>
-      </c>
-      <c r="F90" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>20220722</v>
-      </c>
-      <c r="B91">
-        <v>2200.7479530000001</v>
-      </c>
-      <c r="C91">
-        <v>2226.38</v>
-      </c>
-      <c r="D91">
-        <f>D92</f>
-        <v>7.1615261163340063E-2</v>
-      </c>
-      <c r="E91">
-        <v>176</v>
-      </c>
-      <c r="F91" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>20220729</v>
-      </c>
-      <c r="B92">
-        <v>2226.06306</v>
-      </c>
-      <c r="C92">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D92">
-        <f>100*(B92-C92)/C92</f>
-        <v>7.1615261163340063E-2</v>
-      </c>
-      <c r="E92">
-        <v>180</v>
-      </c>
-      <c r="F92" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>20220802</v>
-      </c>
-      <c r="B93">
-        <v>2220.3086600000001</v>
-      </c>
-      <c r="C93">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D93">
-        <f>100*(B93-C93)/C93</f>
-        <v>-0.18707107760498703</v>
-      </c>
-      <c r="E93">
-        <v>180</v>
-      </c>
-      <c r="F93" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>20220825</v>
-      </c>
-      <c r="B94" s="2">
-        <v>2198.6440400000001</v>
+        <v>20220520</v>
+      </c>
+      <c r="B94">
+        <v>2186.4438722667401</v>
       </c>
       <c r="C94">
         <v>2224.4699999999998</v>
       </c>
       <c r="D94">
-        <f>100*(B94-C94)/C94</f>
-        <v>-1.16099385471594</v>
+        <f t="shared" si="7"/>
+        <v>-1.709446642717579</v>
       </c>
       <c r="E94">
         <v>180</v>
       </c>
       <c r="F94" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>20220831</v>
+        <v>20220608</v>
       </c>
       <c r="B95">
-        <v>2210.5472799999998</v>
+        <v>2228.8510392501998</v>
       </c>
       <c r="C95">
         <v>2224.4699999999998</v>
       </c>
       <c r="D95">
         <f>100*(B95-C95)/C95</f>
+        <v>0.19694755380832502</v>
+      </c>
+      <c r="E95">
+        <v>180</v>
+      </c>
+      <c r="F95" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>20220621</v>
+      </c>
+      <c r="B96">
+        <v>2209.9655012584599</v>
+      </c>
+      <c r="C96">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D96">
+        <f t="shared" ref="D96:D98" si="8">100*(B96-C96)/C96</f>
+        <v>-0.65204290197394976</v>
+      </c>
+      <c r="E96">
+        <v>180</v>
+      </c>
+      <c r="F96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>20220629</v>
+      </c>
+      <c r="B97">
+        <v>2209.2779999999998</v>
+      </c>
+      <c r="C97">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="8"/>
+        <v>-0.68294919688734879</v>
+      </c>
+      <c r="E97">
+        <v>180</v>
+      </c>
+      <c r="F97" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>20220712</v>
+      </c>
+      <c r="B98">
+        <v>2211.98</v>
+      </c>
+      <c r="C98">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="8"/>
+        <v>-0.56148206089539454</v>
+      </c>
+      <c r="E98">
+        <v>180</v>
+      </c>
+      <c r="F98" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>20220720</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2208.6642099999999</v>
+      </c>
+      <c r="C99">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D99">
+        <f>100*(B99-C99)/C99</f>
+        <v>-0.7105418369319384</v>
+      </c>
+      <c r="E99">
+        <v>180</v>
+      </c>
+      <c r="F99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>20220722</v>
+      </c>
+      <c r="B100" s="1">
+        <v>2217.8699700000002</v>
+      </c>
+      <c r="C100">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D100">
+        <f>100*(B100-C100)/C100</f>
+        <v>-0.29670123669906118</v>
+      </c>
+      <c r="E100">
+        <v>180</v>
+      </c>
+      <c r="F100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>20220722</v>
+      </c>
+      <c r="B101">
+        <v>2217.323202</v>
+      </c>
+      <c r="C101">
+        <v>2226.38</v>
+      </c>
+      <c r="D101">
+        <f>100*(B101-C101)/C101</f>
+        <v>-0.40679479693493792</v>
+      </c>
+      <c r="E101">
+        <v>176</v>
+      </c>
+      <c r="F101" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>20220722</v>
+      </c>
+      <c r="B102">
+        <v>2215.267906</v>
+      </c>
+      <c r="C102">
+        <v>2226.38</v>
+      </c>
+      <c r="D102">
+        <f t="shared" ref="D102" si="9">100*(B102-C102)/C102</f>
+        <v>-0.49911039445198346</v>
+      </c>
+      <c r="E102">
+        <v>176</v>
+      </c>
+      <c r="F102" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>20220722</v>
+      </c>
+      <c r="B103">
+        <v>2200.7479530000001</v>
+      </c>
+      <c r="C103">
+        <v>2226.38</v>
+      </c>
+      <c r="D103">
+        <f>D105</f>
+        <v>7.1615261163340063E-2</v>
+      </c>
+      <c r="E103">
+        <v>176</v>
+      </c>
+      <c r="F103" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>20220723</v>
+      </c>
+      <c r="B104" s="3">
+        <v>2210.2288970017398</v>
+      </c>
+      <c r="C104">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D104">
+        <f t="shared" ref="D104" si="10">100*(B104-C104)/C104</f>
+        <v>-0.64020207052736056</v>
+      </c>
+      <c r="E104">
+        <v>180</v>
+      </c>
+      <c r="F104" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>20220729</v>
+      </c>
+      <c r="B105">
+        <v>2226.06306</v>
+      </c>
+      <c r="C105">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D105">
+        <f t="shared" ref="D105:D120" si="11">100*(B105-C105)/C105</f>
+        <v>7.1615261163340063E-2</v>
+      </c>
+      <c r="E105">
+        <v>180</v>
+      </c>
+      <c r="F105" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>20220731</v>
+      </c>
+      <c r="B106">
+        <v>2227.9749999999999</v>
+      </c>
+      <c r="C106">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="11"/>
+        <v>0.15756562237297467</v>
+      </c>
+      <c r="E106">
+        <v>180</v>
+      </c>
+      <c r="F106" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>20220802</v>
+      </c>
+      <c r="B107">
+        <v>2220.3086600000001</v>
+      </c>
+      <c r="C107">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="11"/>
+        <v>-0.18707107760498703</v>
+      </c>
+      <c r="E107">
+        <v>180</v>
+      </c>
+      <c r="F107" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>20220805</v>
+      </c>
+      <c r="B108">
+        <v>2219.8236287263899</v>
+      </c>
+      <c r="C108">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="11"/>
+        <v>-0.20887542981518878</v>
+      </c>
+      <c r="E108">
+        <v>180</v>
+      </c>
+      <c r="F108" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>20220825</v>
+      </c>
+      <c r="B109" s="2">
+        <v>2198.6440400000001</v>
+      </c>
+      <c r="C109">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="11"/>
+        <v>-1.16099385471594</v>
+      </c>
+      <c r="E109">
+        <v>180</v>
+      </c>
+      <c r="F109" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>20220831</v>
+      </c>
+      <c r="B110">
+        <v>2210.5472799999998</v>
+      </c>
+      <c r="C110">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="11"/>
         <v>-0.62588931295994232</v>
       </c>
-      <c r="E95">
-        <v>180</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E110">
+        <v>180</v>
+      </c>
+      <c r="F110" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>20220903</v>
+      </c>
+      <c r="B111">
+        <v>2209.65328484982</v>
+      </c>
+      <c r="C111">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="11"/>
+        <v>-0.66607844341257871</v>
+      </c>
+      <c r="E111">
+        <v>180</v>
+      </c>
+      <c r="F111" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>20220908</v>
+      </c>
+      <c r="B112">
+        <v>2263.1208099999999</v>
+      </c>
+      <c r="C112">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="11"/>
+        <v>1.7375289394777227</v>
+      </c>
+      <c r="E112">
+        <v>180</v>
+      </c>
+      <c r="F112" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>20220914</v>
+      </c>
+      <c r="B113">
+        <v>2221.37</v>
+      </c>
+      <c r="C113">
+        <v>2226.38</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="11"/>
+        <v>-0.22502897079565115</v>
+      </c>
+      <c r="E113">
+        <v>176</v>
+      </c>
+      <c r="F113" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>20220916</v>
+      </c>
+      <c r="B114">
+        <v>2193.7814232117898</v>
+      </c>
+      <c r="C114">
+        <v>2226.38</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="11"/>
+        <v>-1.4641964439228823</v>
+      </c>
+      <c r="E114" t="s">
+        <v>31</v>
+      </c>
+      <c r="F114" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>20220916</v>
+      </c>
+      <c r="B115">
+        <v>2194.6040582389001</v>
+      </c>
+      <c r="C115">
+        <v>2226.38</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="11"/>
+        <v>-1.4272470001122923</v>
+      </c>
+      <c r="E115" t="s">
+        <v>32</v>
+      </c>
+      <c r="F115" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>20220930</v>
+      </c>
+      <c r="B116">
+        <v>2219.7338900066802</v>
+      </c>
+      <c r="C116">
+        <v>2226.38</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="11"/>
+        <v>-0.29851642546734591</v>
+      </c>
+      <c r="E116">
+        <v>176</v>
+      </c>
+      <c r="F116" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>20220930</v>
+      </c>
+      <c r="B117">
+        <v>2210.1862615120499</v>
+      </c>
+      <c r="C117">
+        <v>2215.13</v>
+      </c>
+      <c r="D117">
+        <f t="shared" si="11"/>
+        <v>-0.22318051256360633</v>
+      </c>
+      <c r="E117">
+        <v>202</v>
+      </c>
+      <c r="F117" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>20230118</v>
+      </c>
+      <c r="B118">
+        <v>2276.5568004565698</v>
+      </c>
+      <c r="C118">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D118">
+        <f t="shared" si="11"/>
+        <v>2.3415375553084563</v>
+      </c>
+      <c r="E118">
+        <v>180</v>
+      </c>
+      <c r="F118" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>20230118</v>
+      </c>
+      <c r="B119">
+        <v>2205.9135813586099</v>
+      </c>
+      <c r="C119">
+        <v>2215.13</v>
+      </c>
+      <c r="D119">
+        <f t="shared" si="11"/>
+        <v>-0.41606671578598958</v>
+      </c>
+      <c r="E119">
+        <v>202</v>
+      </c>
+      <c r="F119" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>20230118</v>
+      </c>
+      <c r="B120">
+        <v>2199.9190495084099</v>
+      </c>
+      <c r="C120">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D120">
+        <f t="shared" si="11"/>
+        <v>-0.69520206975020604</v>
+      </c>
+      <c r="E120">
+        <v>196</v>
+      </c>
+      <c r="F120" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LZ Blue Tank Titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C65B2F-FF2D-44E9-94EA-5C3B8A0AAD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AEC5D8-758A-47C9-B227-AA5FCCD966E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14490" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="45" windowWidth="12540" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -1008,7 +1008,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1016,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+      <selection activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,7 +3224,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D105">
-        <f t="shared" ref="D105:D120" si="11">100*(B105-C105)/C105</f>
+        <f t="shared" ref="D105:D121" si="11">100*(B105-C105)/C105</f>
         <v>7.1615261163340063E-2</v>
       </c>
       <c r="E105">
@@ -3546,6 +3546,27 @@
         <v>196</v>
       </c>
       <c r="F120" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>20230221</v>
+      </c>
+      <c r="B121">
+        <v>2191.1105299999999</v>
+      </c>
+      <c r="C121">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="11"/>
+        <v>-1.0928204503187005</v>
+      </c>
+      <c r="E121">
+        <v>196</v>
+      </c>
+      <c r="F121" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lz CBLS aquarium titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AEC5D8-758A-47C9-B227-AA5FCCD966E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CF6CD5-5442-4A0B-90EC-49F75796F177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="45" windowWidth="12540" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="765" windowWidth="13515" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -1008,7 +1008,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1016,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="G121" sqref="G121"/>
+      <selection activeCell="F121" sqref="F121:F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,7 +3224,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D105">
-        <f t="shared" ref="D105:D121" si="11">100*(B105-C105)/C105</f>
+        <f t="shared" ref="D105:D122" si="11">100*(B105-C105)/C105</f>
         <v>7.1615261163340063E-2</v>
       </c>
       <c r="E105">
@@ -3567,6 +3567,27 @@
         <v>196</v>
       </c>
       <c r="F121" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>20230412</v>
+      </c>
+      <c r="B122">
+        <v>2206.5646200000001</v>
+      </c>
+      <c r="C122">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="11"/>
+        <v>-0.39521965223985966</v>
+      </c>
+      <c r="E122">
+        <v>196</v>
+      </c>
+      <c r="F122" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated titrator alkalinity parsing for cbls so that output TA file goes to CBLS lab repo
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CF6CD5-5442-4A0B-90EC-49F75796F177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DF5A77-E08D-454E-9534-39CAE9D784C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="765" windowWidth="13515" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>CRM OPENED 20220908 (Don't recommend using this Batch bottle)</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20230511</t>
   </si>
 </sst>
 </file>
@@ -1016,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121:F122"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3224,7 +3227,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D105">
-        <f t="shared" ref="D105:D122" si="11">100*(B105-C105)/C105</f>
+        <f t="shared" ref="D105:D130" si="11">100*(B105-C105)/C105</f>
         <v>7.1615261163340063E-2</v>
       </c>
       <c r="E105">
@@ -3589,6 +3592,153 @@
       </c>
       <c r="F122" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>20230516</v>
+      </c>
+      <c r="B123">
+        <v>2238.4775300000001</v>
+      </c>
+      <c r="C123">
+        <v>2226.38</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="11"/>
+        <v>0.54337220061265401</v>
+      </c>
+      <c r="E123">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>20230522</v>
+      </c>
+      <c r="B124">
+        <v>2235.8562700000002</v>
+      </c>
+      <c r="C124">
+        <v>2226.38</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="11"/>
+        <v>0.42563578544543668</v>
+      </c>
+      <c r="E124">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>20230523</v>
+      </c>
+      <c r="B125">
+        <v>2228.1219700000001</v>
+      </c>
+      <c r="C125">
+        <v>2226.38</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="11"/>
+        <v>7.8242258733910539E-2</v>
+      </c>
+      <c r="E125">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>20230525</v>
+      </c>
+      <c r="B126">
+        <v>2231.06837</v>
+      </c>
+      <c r="C126">
+        <v>2226.38</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="11"/>
+        <v>0.21058264986210123</v>
+      </c>
+      <c r="E126">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>20230530</v>
+      </c>
+      <c r="B127">
+        <v>2227.05548</v>
+      </c>
+      <c r="C127">
+        <v>2226.38</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="11"/>
+        <v>3.0339834170262016E-2</v>
+      </c>
+      <c r="E127">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>20230531</v>
+      </c>
+      <c r="B128">
+        <v>2220.5585700000001</v>
+      </c>
+      <c r="C128">
+        <v>2226.38</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="11"/>
+        <v>-0.26147513003170902</v>
+      </c>
+      <c r="E128">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>20230601</v>
+      </c>
+      <c r="B129">
+        <v>2244.2638299999999</v>
+      </c>
+      <c r="C129">
+        <v>2226.38</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="11"/>
+        <v>0.80326943289105013</v>
+      </c>
+      <c r="E129">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>20230623</v>
+      </c>
+      <c r="B130" s="1">
+        <v>2223.05278</v>
+      </c>
+      <c r="C130">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D130">
+        <f t="shared" si="11"/>
+        <v>0.34905927811782589</v>
+      </c>
+      <c r="E130">
+        <v>196</v>
+      </c>
+      <c r="F130" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add titration run 0713
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DF5A77-E08D-454E-9534-39CAE9D784C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7EDE86C-CCD5-464A-9CC5-97D9E7772C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9465" yWindow="750" windowWidth="12975" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>CRM OPENED 20230511</t>
+  </si>
+  <si>
+    <t>CRM OPENED 20230512</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F130"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3741,6 +3744,27 @@
         <v>41</v>
       </c>
     </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>20230713</v>
+      </c>
+      <c r="B131">
+        <v>2217.116</v>
+      </c>
+      <c r="C131">
+        <v>2216.3200000000002</v>
+      </c>
+      <c r="D131">
+        <f t="shared" ref="D131" si="12">100*(B131-C131)/C131</f>
+        <v>3.591539127922961E-2</v>
+      </c>
+      <c r="E131">
+        <v>196</v>
+      </c>
+      <c r="F131" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
crm checked with script
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36586BE-C2A8-408D-B314-7E5FDDF76278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFF3947-9B6D-7B44-AD67-CD3A42BF0EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="270" windowWidth="17895" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6580" yWindow="500" windowWidth="17900" windowHeight="9520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -167,14 +167,17 @@
     <t>196 CRM is out, started using 176</t>
   </si>
   <si>
-    <t>CRM 196_202402021_DMB</t>
+    <t>CRM 196_20240215_DMB</t>
+  </si>
+  <si>
+    <t>CRM 196_20240201_DMB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +335,13 @@
       <color rgb="FF4D4D4C"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -675,7 +685,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -683,6 +693,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1038,21 +1049,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20210218</v>
       </c>
@@ -1093,7 +1104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20210221</v>
       </c>
@@ -1114,7 +1125,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20210228</v>
       </c>
@@ -1135,7 +1146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20210228</v>
       </c>
@@ -1156,7 +1167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20210228</v>
       </c>
@@ -1177,7 +1188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20210228</v>
       </c>
@@ -1198,7 +1209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20210228</v>
       </c>
@@ -1219,7 +1230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20210228</v>
       </c>
@@ -1240,7 +1251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20210228</v>
       </c>
@@ -1261,7 +1272,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20210228</v>
       </c>
@@ -1282,7 +1293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20210314</v>
       </c>
@@ -1303,7 +1314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20210314</v>
       </c>
@@ -1324,7 +1335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20210314</v>
       </c>
@@ -1345,7 +1356,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20210314</v>
       </c>
@@ -1366,7 +1377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20210314</v>
       </c>
@@ -1387,7 +1398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20210314</v>
       </c>
@@ -1408,7 +1419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20210314</v>
       </c>
@@ -1429,7 +1440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20210314</v>
       </c>
@@ -1450,7 +1461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20210314</v>
       </c>
@@ -1471,7 +1482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20210314</v>
       </c>
@@ -1492,7 +1503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20210314</v>
       </c>
@@ -1513,7 +1524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20210314</v>
       </c>
@@ -1534,7 +1545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20210328</v>
       </c>
@@ -1555,7 +1566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20210328</v>
       </c>
@@ -1576,7 +1587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20210328</v>
       </c>
@@ -1597,7 +1608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20210328</v>
       </c>
@@ -1618,7 +1629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20210328</v>
       </c>
@@ -1639,7 +1650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20210404</v>
       </c>
@@ -1660,7 +1671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20210418</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20210428</v>
       </c>
@@ -1702,7 +1713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20210504</v>
       </c>
@@ -1723,7 +1734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20210505</v>
       </c>
@@ -1744,7 +1755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20210506</v>
       </c>
@@ -1765,7 +1776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20210511</v>
       </c>
@@ -1786,7 +1797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>20210525</v>
       </c>
@@ -1807,7 +1818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>20210526</v>
       </c>
@@ -1828,7 +1839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20210527</v>
       </c>
@@ -1849,7 +1860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>20210601</v>
       </c>
@@ -1870,7 +1881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>20210603</v>
       </c>
@@ -1891,7 +1902,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>20210610</v>
       </c>
@@ -1912,7 +1923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>20210615</v>
       </c>
@@ -1933,7 +1944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>20210624</v>
       </c>
@@ -1954,7 +1965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>20210706</v>
       </c>
@@ -1975,7 +1986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>20210708</v>
       </c>
@@ -1996,7 +2007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>20210715</v>
       </c>
@@ -2017,7 +2028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>20210719</v>
       </c>
@@ -2038,7 +2049,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>20210723</v>
       </c>
@@ -2059,7 +2070,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>20210724</v>
       </c>
@@ -2080,7 +2091,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>20210730</v>
       </c>
@@ -2101,7 +2112,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>20210811</v>
       </c>
@@ -2122,7 +2133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>20211018</v>
       </c>
@@ -2143,7 +2154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>20211110</v>
       </c>
@@ -2164,7 +2175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>20211117</v>
       </c>
@@ -2185,7 +2196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>20211206</v>
       </c>
@@ -2206,7 +2217,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>20220118</v>
       </c>
@@ -2227,7 +2238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>20220127</v>
       </c>
@@ -2248,7 +2259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>20220131</v>
       </c>
@@ -2269,7 +2280,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>20220201</v>
       </c>
@@ -2290,7 +2301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>20220203</v>
       </c>
@@ -2311,7 +2322,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>20220209</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>20220210</v>
       </c>
@@ -2353,7 +2364,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>20220216</v>
       </c>
@@ -2374,7 +2385,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>20220224</v>
       </c>
@@ -2395,7 +2406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>20220302</v>
       </c>
@@ -2416,7 +2427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>20220303</v>
       </c>
@@ -2437,7 +2448,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>20220308</v>
       </c>
@@ -2458,7 +2469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>20220309</v>
       </c>
@@ -2479,7 +2490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>20220310</v>
       </c>
@@ -2500,7 +2511,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>20220311</v>
       </c>
@@ -2521,7 +2532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>20220314</v>
       </c>
@@ -2542,7 +2553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>20220315</v>
       </c>
@@ -2563,7 +2574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>20220317</v>
       </c>
@@ -2584,7 +2595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>20220318</v>
       </c>
@@ -2605,7 +2616,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>20220321</v>
       </c>
@@ -2626,7 +2637,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>20220322</v>
       </c>
@@ -2647,7 +2658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>20220323</v>
       </c>
@@ -2668,7 +2679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>20220324</v>
       </c>
@@ -2689,7 +2700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>20220329</v>
       </c>
@@ -2710,7 +2721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>20220330</v>
       </c>
@@ -2731,7 +2742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>20220331</v>
       </c>
@@ -2752,7 +2763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>20220401</v>
       </c>
@@ -2773,7 +2784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>20220404</v>
       </c>
@@ -2794,7 +2805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>20220405</v>
       </c>
@@ -2815,7 +2826,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>20220406</v>
       </c>
@@ -2836,7 +2847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>20220407</v>
       </c>
@@ -2857,7 +2868,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>20220408</v>
       </c>
@@ -2878,7 +2889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>20220413</v>
       </c>
@@ -2899,7 +2910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>20220415</v>
       </c>
@@ -2920,7 +2931,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>20220420</v>
       </c>
@@ -2941,7 +2952,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>20220427</v>
       </c>
@@ -2962,7 +2973,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>20220504</v>
       </c>
@@ -2983,7 +2994,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>20220518</v>
       </c>
@@ -3004,7 +3015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>20220520</v>
       </c>
@@ -3025,7 +3036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>20220608</v>
       </c>
@@ -3046,7 +3057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>20220621</v>
       </c>
@@ -3067,7 +3078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>20220629</v>
       </c>
@@ -3088,7 +3099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>20220712</v>
       </c>
@@ -3109,7 +3120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>20220720</v>
       </c>
@@ -3130,7 +3141,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>20220722</v>
       </c>
@@ -3151,7 +3162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>20220722</v>
       </c>
@@ -3172,7 +3183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>20220722</v>
       </c>
@@ -3193,7 +3204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>20220722</v>
       </c>
@@ -3214,7 +3225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>20220723</v>
       </c>
@@ -3235,7 +3246,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>20220729</v>
       </c>
@@ -3256,7 +3267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>20220731</v>
       </c>
@@ -3277,7 +3288,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>20220802</v>
       </c>
@@ -3298,7 +3309,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>20220805</v>
       </c>
@@ -3319,7 +3330,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>20220825</v>
       </c>
@@ -3340,7 +3351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>20220831</v>
       </c>
@@ -3361,7 +3372,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>20220903</v>
       </c>
@@ -3382,7 +3393,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>20220908</v>
       </c>
@@ -3403,7 +3414,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>20220914</v>
       </c>
@@ -3424,7 +3435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>20220916</v>
       </c>
@@ -3445,7 +3456,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>20220916</v>
       </c>
@@ -3466,7 +3477,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>20220930</v>
       </c>
@@ -3487,7 +3498,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>20220930</v>
       </c>
@@ -3508,7 +3519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>20230118</v>
       </c>
@@ -3529,7 +3540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>20230118</v>
       </c>
@@ -3550,7 +3561,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>20230118</v>
       </c>
@@ -3571,7 +3582,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>20230221</v>
       </c>
@@ -3592,7 +3603,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>20230412</v>
       </c>
@@ -3613,7 +3624,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>20230516</v>
       </c>
@@ -3631,7 +3642,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>20230522</v>
       </c>
@@ -3649,7 +3660,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>20230523</v>
       </c>
@@ -3667,7 +3678,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>20230525</v>
       </c>
@@ -3685,7 +3696,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>20230530</v>
       </c>
@@ -3703,7 +3714,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>20230531</v>
       </c>
@@ -3721,7 +3732,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>20230601</v>
       </c>
@@ -3739,7 +3750,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>20230623</v>
       </c>
@@ -3760,7 +3771,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>20230713</v>
       </c>
@@ -3771,7 +3782,7 @@
         <v>2216.3200000000002</v>
       </c>
       <c r="D131">
-        <f t="shared" ref="D131:D135" si="12">100*(B131-C131)/C131</f>
+        <f t="shared" ref="D131:D136" si="12">100*(B131-C131)/C131</f>
         <v>3.591539127922961E-2</v>
       </c>
       <c r="E131">
@@ -3781,7 +3792,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>20231103</v>
       </c>
@@ -3799,7 +3810,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>20231110</v>
       </c>
@@ -3820,7 +3831,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>20231116</v>
       </c>
@@ -3838,7 +3849,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>20240201</v>
       </c>
@@ -3856,6 +3867,27 @@
         <v>196</v>
       </c>
       <c r="F135" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>20240215</v>
+      </c>
+      <c r="B136" s="5">
+        <v>2230.9595899999999</v>
+      </c>
+      <c r="C136">
+        <v>2215.36</v>
+      </c>
+      <c r="D136">
+        <f t="shared" si="12"/>
+        <v>0.70415598367758769</v>
+      </c>
+      <c r="E136">
+        <v>196</v>
+      </c>
+      <c r="F136" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran CRM for 0320 titraations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8294A7-1FA8-EA4F-BB70-C5F0C5CADD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371E0D7C-A953-874B-8B1A-74A2A9894B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="500" windowWidth="17900" windowHeight="9520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -180,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,26 +322,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4D4D4C"/>
-      <name val="Lucida Grande"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -688,15 +669,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -756,9 +735,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -796,7 +775,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -902,7 +881,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1044,7 +1023,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1052,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1066,2852 +1045,2882 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>20210218</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2215.547681</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>100*(B2-C2)/C2</f>
         <v>-0.82908409315733844</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>141</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>20210221</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2215.5540000000001</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>100*(B3-C3)/C3</f>
         <v>-0.82880124615612205</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>141</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>20210228</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2211.1392636523301</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" ref="D4:D11" si="0">100*(B4-C4)/C4</f>
         <v>-1.0264108263246032</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>141</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>20210228</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2213.5992626297498</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>-0.91629793919843106</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>141</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>20210228</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>2218.8110320871701</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>-0.68301207718782442</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>141</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>20210228</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>2208.8304250821302</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>-1.1297575688259525</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>141</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>20210228</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>2203.4973775284002</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>-1.3684720027393935</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>141</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>20210228</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>2213.3549756320699</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>-0.9272325561835687</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>141</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>20210228</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>2230.9452295190799</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>-0.13986896027967938</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>141</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>20210228</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>2222.5457646464001</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>-0.515840387883998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>141</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>20210314</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>2182.6919702618002</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <f t="shared" ref="D12:D23" si="1">100*(B12-C12)/C12</f>
         <v>-2.2997502199214876</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>141</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>20210314</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>2183.0707049272701</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>-2.2827975431714354</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>141</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>20210314</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>2179.9893168764502</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>-2.4207246471037158</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>141</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>20210314</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>2180.1189155137999</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>-2.4149236365109514</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>141</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>20210314</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>2194.2628893932401</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>-1.7818202028924801</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>141</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>20210314</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>2194.8087986166001</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <f t="shared" si="1"/>
         <v>-1.7573845664370418</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>141</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>20210314</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>2192.1340883392099</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <f t="shared" si="1"/>
         <v>-1.8771082222486413</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>141</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>20210314</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>2192.25361055657</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>2234.0700000000002</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <f t="shared" si="1"/>
         <v>-1.8717582458665181</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>141</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
         <v>20210314</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>2205.7312106719601</v>
       </c>
-      <c r="C20">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D20" s="1">
         <f t="shared" si="1"/>
         <v>-0.84239343879844331</v>
       </c>
-      <c r="E20">
-        <v>180</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="1">
+        <v>180</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>20210314</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>2194.00552102248</v>
       </c>
-      <c r="C21">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D21">
+      <c r="C21" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D21" s="1">
         <f t="shared" si="1"/>
         <v>-1.3695162882628122</v>
       </c>
-      <c r="E21">
-        <v>180</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="1">
+        <v>180</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>20210314</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>2192.0447529285698</v>
       </c>
-      <c r="C22">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D22" s="1">
         <f t="shared" si="1"/>
         <v>-1.4576616934114655</v>
       </c>
-      <c r="E22">
-        <v>180</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="1">
+        <v>180</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>20210314</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>2196.3789375564002</v>
       </c>
-      <c r="C23">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D23" s="1">
         <f t="shared" si="1"/>
         <v>-1.2628204670595531</v>
       </c>
-      <c r="E23">
-        <v>180</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E23" s="1">
+        <v>180</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>20210328</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>2226.22004515256</v>
       </c>
-      <c r="C24">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D24" s="1">
         <f t="shared" ref="D24:D28" si="2">100*(B24-C24)/C24</f>
         <v>7.8672454677304396E-2</v>
       </c>
-      <c r="E24">
-        <v>180</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="1">
+        <v>180</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>20210328</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>2224.4256267383998</v>
       </c>
-      <c r="C25">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D25" s="1">
         <f t="shared" si="2"/>
         <v>-1.9947790529860109E-3</v>
       </c>
-      <c r="E25">
-        <v>180</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25" s="1">
+        <v>180</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>20210328</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>2224.2019706982401</v>
       </c>
-      <c r="C26">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D26" s="1">
         <f t="shared" si="2"/>
         <v>-1.2049130883299172E-2</v>
       </c>
-      <c r="E26">
-        <v>180</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="1">
+        <v>180</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>20210328</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>2225.54963650217</v>
       </c>
-      <c r="C27">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D27" s="1">
         <f t="shared" si="2"/>
         <v>4.8534549900432933E-2</v>
       </c>
-      <c r="E27">
-        <v>180</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27" s="1">
+        <v>180</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>20210328</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>2228.2924875591002</v>
       </c>
-      <c r="C28">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D28" s="1">
         <f t="shared" si="2"/>
         <v>0.17183812589517547</v>
       </c>
-      <c r="E28">
-        <v>180</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E28" s="1">
+        <v>180</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>20210404</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>2272.8870000000002</v>
       </c>
-      <c r="C29">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D29" s="1">
         <f t="shared" ref="D29:D30" si="3">100*(B29-C29)/C29</f>
         <v>2.1765634061147319</v>
       </c>
-      <c r="E29">
-        <v>180</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="E29" s="1">
+        <v>180</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>20210418</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>2218.2559999999999</v>
       </c>
-      <c r="C30">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D30" s="1">
         <f t="shared" si="3"/>
         <v>-0.27934744006437229</v>
       </c>
-      <c r="E30">
-        <v>180</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E30" s="1">
+        <v>180</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>20210428</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>2223.7829999999999</v>
       </c>
-      <c r="C31">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D31" s="1">
         <f t="shared" ref="D31:D39" si="4">100*(B31-C31)/C31</f>
         <v>-3.0883761075667381E-2</v>
       </c>
-      <c r="E31">
-        <v>180</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="E31" s="1">
+        <v>180</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
         <v>20210504</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>2224.8229999999999</v>
       </c>
-      <c r="C32">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D32" s="1">
         <f t="shared" si="4"/>
         <v>1.5868948558535989E-2</v>
       </c>
-      <c r="E32">
-        <v>180</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="E32" s="1">
+        <v>180</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
         <v>20210505</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>2229.0880000000002</v>
       </c>
-      <c r="C33">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D33" s="1">
         <f t="shared" si="4"/>
         <v>0.20760001258728566</v>
       </c>
-      <c r="E33">
-        <v>180</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="E33" s="1">
+        <v>180</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
         <v>20210506</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>2225.0940000000001</v>
       </c>
-      <c r="C34">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D34" s="1">
         <f t="shared" si="4"/>
         <v>2.8051625780534287E-2</v>
       </c>
-      <c r="E34">
-        <v>180</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E34" s="1">
+        <v>180</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
         <v>20210511</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>2228.8789999999999</v>
       </c>
-      <c r="C35">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D35" s="1">
         <f t="shared" si="4"/>
         <v>0.19820451613193732</v>
       </c>
-      <c r="E35">
-        <v>180</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="E35" s="1">
+        <v>180</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>20210525</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>2223.5051632014602</v>
       </c>
-      <c r="C36">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D36">
+      <c r="C36" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D36" s="1">
         <f t="shared" si="4"/>
         <v>-4.337378335242266E-2</v>
       </c>
-      <c r="E36">
-        <v>180</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="E36" s="1">
+        <v>180</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>20210526</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>2223.4699999999998</v>
       </c>
-      <c r="C37">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D37">
+      <c r="C37" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D37" s="1">
         <f t="shared" si="4"/>
         <v>-4.4954528494427888E-2</v>
       </c>
-      <c r="E37">
-        <v>180</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="E37" s="1">
+        <v>180</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>20210527</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>2221.3470000000002</v>
       </c>
-      <c r="C38">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D38">
+      <c r="C38" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D38" s="1">
         <f t="shared" si="4"/>
         <v>-0.14039299248807999</v>
       </c>
-      <c r="E38">
-        <v>180</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="E38" s="1">
+        <v>180</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>20210601</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>2222.2813428003801</v>
       </c>
-      <c r="C39">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D39">
+      <c r="C39" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D39" s="1">
         <f t="shared" si="4"/>
         <v>-9.8390052444837811E-2</v>
       </c>
-      <c r="E39">
-        <v>180</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E39" s="1">
+        <v>180</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>20210603</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>2228.9667413407301</v>
       </c>
-      <c r="C40">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D40">
+      <c r="C40" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D40" s="1">
         <f t="shared" ref="D40:D51" si="5">100*(B40-C40)/C40</f>
         <v>0.20214888673393194</v>
       </c>
-      <c r="E40">
-        <v>180</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E40" s="1">
+        <v>180</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
+    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>20210610</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>2229.3150000000001</v>
       </c>
-      <c r="C41">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D41">
+      <c r="C41" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D41" s="1">
         <f t="shared" si="5"/>
         <v>0.21780469055551457</v>
       </c>
-      <c r="E41">
-        <v>180</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E41" s="1">
+        <v>180</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
+    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>20210615</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>2228.7220000000002</v>
       </c>
-      <c r="C42">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D42">
+      <c r="C42" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D42" s="1">
         <f t="shared" si="5"/>
         <v>0.19114665515832571</v>
       </c>
-      <c r="E42">
-        <v>180</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="E42" s="1">
+        <v>180</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
+    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
         <v>20210624</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>2228.4520000000002</v>
       </c>
-      <c r="C43">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D43">
+      <c r="C43" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D43" s="1">
         <f t="shared" si="5"/>
         <v>0.17900893246483099</v>
       </c>
-      <c r="E43">
-        <v>180</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="E43" s="1">
+        <v>180</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
+    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>20210706</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>2230.0918634412801</v>
       </c>
-      <c r="C44">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D44">
+      <c r="C44" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D44" s="1">
         <f t="shared" si="5"/>
         <v>0.25272822026281822</v>
       </c>
-      <c r="E44">
-        <v>180</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E44" s="1">
+        <v>180</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
+    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>20210708</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>2228.9570833859798</v>
       </c>
-      <c r="C45">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D45">
+      <c r="C45" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D45" s="1">
         <f t="shared" si="5"/>
         <v>0.20171471793191126</v>
       </c>
-      <c r="E45">
-        <v>180</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E45" s="1">
+        <v>180</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46">
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>20210715</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>2230.4602923572402</v>
       </c>
-      <c r="C46">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D46" s="1">
         <f t="shared" si="5"/>
         <v>0.26929076846351618</v>
       </c>
-      <c r="E46">
-        <v>180</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="E46" s="1">
+        <v>180</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>20210719</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>2226.4870498855298</v>
       </c>
-      <c r="C47">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D47">
+      <c r="C47" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D47" s="1">
         <f t="shared" si="5"/>
         <v>9.0675526553741517E-2</v>
       </c>
-      <c r="E47">
-        <v>180</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="E47" s="1">
+        <v>180</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48">
+    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>20210723</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>2231.0569999999998</v>
       </c>
-      <c r="C48">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D48">
+      <c r="C48" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D48" s="1">
         <f t="shared" si="5"/>
         <v>0.29611547919279602</v>
       </c>
-      <c r="E48">
-        <v>180</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E48" s="1">
+        <v>180</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49">
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>20210724</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>2227.3916066216202</v>
       </c>
-      <c r="C49">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D49">
+      <c r="C49" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D49" s="1">
         <f t="shared" si="5"/>
         <v>0.13133944812114404</v>
       </c>
-      <c r="E49">
-        <v>180</v>
-      </c>
-      <c r="F49" t="s">
+      <c r="E49" s="1">
+        <v>180</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>20210730</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>2225.6402336351998</v>
       </c>
-      <c r="C50">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D50">
+      <c r="C50" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D50" s="1">
         <f t="shared" si="5"/>
         <v>5.2607301298737238E-2</v>
       </c>
-      <c r="E50">
-        <v>180</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E50" s="1">
+        <v>180</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>20210811</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>2221.0572992288098</v>
       </c>
-      <c r="C51">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D51">
+      <c r="C51" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D51" s="1">
         <f t="shared" si="5"/>
         <v>-0.15341635406141577</v>
       </c>
-      <c r="E51">
-        <v>180</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E51" s="1">
+        <v>180</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52">
+    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>20211018</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>2221.73708567331</v>
       </c>
-      <c r="C52">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D52">
+      <c r="C52" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D52" s="1">
         <f t="shared" ref="D52:D74" si="6">100*(B52-C52)/C52</f>
         <v>-0.12285687497200466</v>
       </c>
-      <c r="E52">
-        <v>180</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="E52" s="1">
+        <v>180</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53">
+    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>20211110</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>2220.49470192943</v>
       </c>
-      <c r="C53">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D53">
+      <c r="C53" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D53" s="1">
         <f t="shared" si="6"/>
         <v>-0.17870765038727457</v>
       </c>
-      <c r="E53">
-        <v>180</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="E53" s="1">
+        <v>180</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54">
+    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
         <v>20211117</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>2231.6860000000001</v>
       </c>
-      <c r="C54">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D54">
+      <c r="C54" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D54" s="1">
         <f t="shared" si="6"/>
         <v>0.32439187761580734</v>
       </c>
-      <c r="E54">
-        <v>180</v>
-      </c>
-      <c r="F54" t="s">
+      <c r="E54" s="1">
+        <v>180</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55">
+    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>20211206</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>2228.1970000000001</v>
       </c>
-      <c r="C55">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D55">
+      <c r="C55" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D55" s="1">
         <f t="shared" si="6"/>
         <v>0.16754552769874698</v>
       </c>
-      <c r="E55">
-        <v>180</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E55" s="1">
+        <v>180</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56">
+    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>20220118</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>2203.6729999999998</v>
       </c>
-      <c r="C56">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D56">
+      <c r="C56" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D56" s="1">
         <f t="shared" si="6"/>
         <v>-0.93491932909861797</v>
       </c>
-      <c r="E56">
-        <v>180</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="E56" s="1">
+        <v>180</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57">
+    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>20220127</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>2231.4175319214601</v>
       </c>
-      <c r="C57">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D57">
+      <c r="C57" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D57" s="1">
         <f t="shared" si="6"/>
         <v>0.31232302172923299</v>
       </c>
-      <c r="E57">
-        <v>180</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="E57" s="1">
+        <v>180</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58">
+    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>20220131</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>2232.37</v>
       </c>
-      <c r="C58">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D58">
+      <c r="C58" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D58" s="1">
         <f t="shared" si="6"/>
         <v>0.35514077510598441</v>
       </c>
-      <c r="E58">
-        <v>180</v>
-      </c>
-      <c r="F58" t="s">
+      <c r="E58" s="1">
+        <v>180</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59">
+    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>20220201</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>2228.2564673073002</v>
       </c>
-      <c r="C59">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D59">
+      <c r="C59" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D59" s="1">
         <f t="shared" si="6"/>
         <v>0.17021885245925669</v>
       </c>
-      <c r="E59">
-        <v>180</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E59" s="1">
+        <v>180</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60">
+    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
         <v>20220203</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>2226.15763917096</v>
       </c>
-      <c r="C60">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D60">
+      <c r="C60" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D60" s="1">
         <f t="shared" si="6"/>
         <v>7.5867023199243433E-2</v>
       </c>
-      <c r="E60">
-        <v>180</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="E60" s="1">
+        <v>180</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61">
+    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>20220209</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>2228.5439999999999</v>
       </c>
-      <c r="C61">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D61">
+      <c r="C61" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D61" s="1">
         <f t="shared" si="6"/>
         <v>0.18314474908630232</v>
       </c>
-      <c r="E61">
-        <v>180</v>
-      </c>
-      <c r="F61" t="s">
+      <c r="E61" s="1">
+        <v>180</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62">
+    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
         <v>20220210</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>2228.61</v>
       </c>
-      <c r="C62">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D62">
+      <c r="C62" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D62" s="1">
         <f t="shared" si="6"/>
         <v>0.18611174796694618</v>
       </c>
-      <c r="E62">
-        <v>180</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="E62" s="1">
+        <v>180</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63">
+    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
         <v>20220216</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>2227.6280000000002</v>
       </c>
-      <c r="C63">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D63">
+      <c r="C63" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D63" s="1">
         <f t="shared" si="6"/>
         <v>0.14196640098541929</v>
       </c>
-      <c r="E63">
-        <v>180</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="E63" s="1">
+        <v>180</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64">
+    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
         <v>20220224</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>2222.0050000000001</v>
       </c>
-      <c r="C64">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D64">
+      <c r="C64" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D64" s="1">
         <f t="shared" si="6"/>
         <v>-0.11081291273875085</v>
       </c>
-      <c r="E64">
-        <v>180</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="E64" s="1">
+        <v>180</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65">
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>20220302</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>2224.779</v>
       </c>
-      <c r="C65">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D65">
+      <c r="C65" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D65" s="1">
         <f t="shared" si="6"/>
         <v>1.3890949304787049E-2</v>
       </c>
-      <c r="E65">
-        <v>180</v>
-      </c>
-      <c r="F65" t="s">
+      <c r="E65" s="1">
+        <v>180</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66">
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
         <v>20220303</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>2221.846</v>
       </c>
-      <c r="C66">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D66">
+      <c r="C66" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D66" s="1">
         <f t="shared" si="6"/>
         <v>-0.11796068276936962</v>
       </c>
-      <c r="E66">
-        <v>180</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E66" s="1">
+        <v>180</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67">
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
         <v>20220308</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>2220.8926944598902</v>
       </c>
-      <c r="C67">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D67">
+      <c r="C67" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D67" s="1">
         <f t="shared" si="6"/>
         <v>-0.16081608383613138</v>
       </c>
-      <c r="E67">
-        <v>180</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E67" s="1">
+        <v>180</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68">
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>20220309</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>2217.547</v>
       </c>
-      <c r="C68">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D68">
+      <c r="C68" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D68" s="1">
         <f t="shared" si="6"/>
         <v>-0.31122020076691415</v>
       </c>
-      <c r="E68">
-        <v>180</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E68" s="1">
+        <v>180</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>20220310</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>2221.9227812661102</v>
       </c>
-      <c r="C69">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D69">
+      <c r="C69" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D69" s="1">
         <f t="shared" si="6"/>
         <v>-0.11450901715418155</v>
       </c>
-      <c r="E69">
-        <v>180</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E69" s="1">
+        <v>180</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70">
+    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
         <v>20220311</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>2226.5838482945901</v>
       </c>
-      <c r="C70">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D70">
+      <c r="C70" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D70" s="1">
         <f t="shared" si="6"/>
         <v>9.5027053392057345E-2</v>
       </c>
-      <c r="E70">
-        <v>180</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E70" s="1">
+        <v>180</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71">
+    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>20220314</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>2221.5278341974199</v>
       </c>
-      <c r="C71">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D71">
+      <c r="C71" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D71" s="1">
         <f t="shared" si="6"/>
         <v>-0.13226367640740913</v>
       </c>
-      <c r="E71">
-        <v>180</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E71" s="1">
+        <v>180</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72">
+    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
         <v>20220315</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>2225.7539999999999</v>
       </c>
-      <c r="C72">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D72">
+      <c r="C72" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D72" s="1">
         <f t="shared" si="6"/>
         <v>5.7721614586850156E-2</v>
       </c>
-      <c r="E72">
-        <v>180</v>
-      </c>
-      <c r="F72" t="s">
+      <c r="E72" s="1">
+        <v>180</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73">
+    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
         <v>20220317</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>2223.0121947257499</v>
       </c>
-      <c r="C73">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D73">
+      <c r="C73" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D73" s="1">
         <f t="shared" si="6"/>
         <v>-6.5534948740596621E-2</v>
       </c>
-      <c r="E73">
-        <v>180</v>
-      </c>
-      <c r="F73" t="s">
+      <c r="E73" s="1">
+        <v>180</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74">
+    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
         <v>20220318</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>2226.3488441921399</v>
       </c>
-      <c r="C74">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D74">
+      <c r="C74" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D74" s="1">
         <f t="shared" si="6"/>
         <v>8.4462554772154724E-2</v>
       </c>
-      <c r="E74">
-        <v>180</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="E74" s="1">
+        <v>180</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75">
+    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
         <v>20220321</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>2224.7499947312399</v>
       </c>
-      <c r="C75">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D75">
+      <c r="C75" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D75" s="1">
         <f t="shared" ref="D75:D94" si="7">100*(B75-C75)/C75</f>
         <v>1.258703112382251E-2</v>
       </c>
-      <c r="E75">
-        <v>180</v>
-      </c>
-      <c r="F75" t="s">
+      <c r="E75" s="1">
+        <v>180</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76">
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
         <v>20220322</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>2223.1790210232102</v>
       </c>
-      <c r="C76">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D76">
+      <c r="C76" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D76" s="1">
         <f t="shared" si="7"/>
         <v>-5.8035351197794287E-2</v>
       </c>
-      <c r="E76">
-        <v>180</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="E76" s="1">
+        <v>180</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77">
+    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
         <v>20220323</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>2227.4597991999999</v>
       </c>
-      <c r="C77">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D77">
+      <c r="C77" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D77" s="1">
         <f t="shared" si="7"/>
         <v>0.13440501332902252</v>
       </c>
-      <c r="E77">
-        <v>180</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="E77" s="1">
+        <v>180</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78">
+    <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
         <v>20220324</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>2220.70646995792</v>
       </c>
-      <c r="C78">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D78">
+      <c r="C78" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D78" s="1">
         <f t="shared" si="7"/>
         <v>-0.16918771851631018</v>
       </c>
-      <c r="E78">
-        <v>180</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="E78" s="1">
+        <v>180</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79">
+    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
         <v>20220329</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>2234.105</v>
       </c>
-      <c r="C79">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D79">
+      <c r="C79" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D79" s="1">
         <f t="shared" si="7"/>
         <v>0.43313688204382256</v>
       </c>
-      <c r="E79">
-        <v>180</v>
-      </c>
-      <c r="F79" t="s">
+      <c r="E79" s="1">
+        <v>180</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80">
+    <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
         <v>20220330</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>2227.7080000000001</v>
       </c>
-      <c r="C80">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D80">
+      <c r="C80" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D80" s="1">
         <f t="shared" si="7"/>
         <v>0.14556276326497025</v>
       </c>
-      <c r="E80">
-        <v>180</v>
-      </c>
-      <c r="F80" t="s">
+      <c r="E80" s="1">
+        <v>180</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81">
+    <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
         <v>20220331</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>2226.165</v>
       </c>
-      <c r="C81">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D81">
+      <c r="C81" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D81" s="1">
         <f t="shared" si="7"/>
         <v>7.619792579806263E-2</v>
       </c>
-      <c r="E81">
-        <v>180</v>
-      </c>
-      <c r="F81" t="s">
+      <c r="E81" s="1">
+        <v>180</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82">
+    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
         <v>20220401</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>2225.92</v>
       </c>
-      <c r="C82">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D82">
+      <c r="C82" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D82" s="1">
         <f t="shared" si="7"/>
         <v>6.5184066316932701E-2</v>
       </c>
-      <c r="E82">
-        <v>180</v>
-      </c>
-      <c r="F82" t="s">
+      <c r="E82" s="1">
+        <v>180</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83">
+    <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
         <v>20220404</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>2224.5797358742998</v>
       </c>
-      <c r="C83">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D83">
+      <c r="C83" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D83" s="1">
         <f t="shared" si="7"/>
         <v>4.9331244880796727E-3</v>
       </c>
-      <c r="E83">
-        <v>180</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="E83" s="1">
+        <v>180</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84">
+    <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
         <v>20220405</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>2221.9426290986098</v>
       </c>
-      <c r="C84">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D84">
+      <c r="C84" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D84" s="1">
         <f t="shared" si="7"/>
         <v>-0.11361676720252403</v>
       </c>
-      <c r="E84">
-        <v>180</v>
-      </c>
-      <c r="F84" t="s">
+      <c r="E84" s="1">
+        <v>180</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85">
+    <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
         <v>20220406</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>2219.3566865192001</v>
       </c>
-      <c r="C85">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D85">
+      <c r="C85" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D85" s="1">
         <f t="shared" si="7"/>
         <v>-0.22986659657355063</v>
       </c>
-      <c r="E85">
-        <v>180</v>
-      </c>
-      <c r="F85" t="s">
+      <c r="E85" s="1">
+        <v>180</v>
+      </c>
+      <c r="F85" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86">
+    <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
         <v>20220407</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>2226.1503724982399</v>
       </c>
-      <c r="C86">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D86">
+      <c r="C86" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D86" s="1">
         <f t="shared" si="7"/>
         <v>7.5540353353387713E-2</v>
       </c>
-      <c r="E86">
-        <v>180</v>
-      </c>
-      <c r="F86" t="s">
+      <c r="E86" s="1">
+        <v>180</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87">
+    <row r="87" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
         <v>20220408</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>2220.60904733079</v>
       </c>
-      <c r="C87">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D87">
+      <c r="C87" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D87" s="1">
         <f t="shared" si="7"/>
         <v>-0.17356730678363105</v>
       </c>
-      <c r="E87">
-        <v>180</v>
-      </c>
-      <c r="F87" t="s">
+      <c r="E87" s="1">
+        <v>180</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88">
+    <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
         <v>20220413</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>2223.6496216999999</v>
       </c>
-      <c r="C88">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D88">
+      <c r="C88" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D88" s="1">
         <f t="shared" si="7"/>
         <v>-3.687971966355591E-2</v>
       </c>
-      <c r="E88">
-        <v>180</v>
-      </c>
-      <c r="F88" t="s">
+      <c r="E88" s="1">
+        <v>180</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89">
+    <row r="89" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
         <v>20220415</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>2223.5663069920402</v>
       </c>
-      <c r="C89">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D89">
+      <c r="C89" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D89" s="1">
         <f t="shared" si="7"/>
         <v>-4.0625093076537153E-2</v>
       </c>
-      <c r="E89">
-        <v>180</v>
-      </c>
-      <c r="F89" t="s">
+      <c r="E89" s="1">
+        <v>180</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90">
+    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
         <v>20220420</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>2225.2184000000002</v>
       </c>
-      <c r="C90">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D90">
+      <c r="C90" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D90" s="1">
         <f t="shared" si="7"/>
         <v>3.3643969125247891E-2</v>
       </c>
-      <c r="E90">
-        <v>180</v>
-      </c>
-      <c r="F90" t="s">
+      <c r="E90" s="1">
+        <v>180</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91">
+    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
         <v>20220427</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>2215.5293579999998</v>
       </c>
-      <c r="C91">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D91">
+      <c r="C91" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D91" s="1">
         <f t="shared" si="7"/>
         <v>-0.40192234554747991</v>
       </c>
-      <c r="E91">
-        <v>180</v>
-      </c>
-      <c r="F91" t="s">
+      <c r="E91" s="1">
+        <v>180</v>
+      </c>
+      <c r="F91" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92">
+    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
         <v>20220504</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>2200.1692800000001</v>
       </c>
-      <c r="C92">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D92">
+      <c r="C92" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D92" s="1">
         <f t="shared" si="7"/>
         <v>-1.0924274096751014</v>
       </c>
-      <c r="E92">
-        <v>180</v>
-      </c>
-      <c r="F92" t="s">
+      <c r="E92" s="1">
+        <v>180</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93">
+    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
         <v>20220518</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>2201.1546499999999</v>
       </c>
-      <c r="C93">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D93">
+      <c r="C93" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D93" s="1">
         <f t="shared" si="7"/>
         <v>-1.0481305659325526</v>
       </c>
-      <c r="E93">
-        <v>180</v>
-      </c>
-      <c r="F93" t="s">
+      <c r="E93" s="1">
+        <v>180</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94">
+    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
         <v>20220520</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>2186.4438722667401</v>
       </c>
-      <c r="C94">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D94">
+      <c r="C94" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D94" s="1">
         <f t="shared" si="7"/>
         <v>-1.709446642717579</v>
       </c>
-      <c r="E94">
-        <v>180</v>
-      </c>
-      <c r="F94" t="s">
+      <c r="E94" s="1">
+        <v>180</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95">
+    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
         <v>20220608</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>2228.8510392501998</v>
       </c>
-      <c r="C95">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D95">
+      <c r="C95" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D95" s="1">
         <f>100*(B95-C95)/C95</f>
         <v>0.19694755380832502</v>
       </c>
-      <c r="E95">
-        <v>180</v>
-      </c>
-      <c r="F95" t="s">
+      <c r="E95" s="1">
+        <v>180</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96">
+    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
         <v>20220621</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>2209.9655012584599</v>
       </c>
-      <c r="C96">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D96">
+      <c r="C96" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D96" s="1">
         <f t="shared" ref="D96:D98" si="8">100*(B96-C96)/C96</f>
         <v>-0.65204290197394976</v>
       </c>
-      <c r="E96">
-        <v>180</v>
-      </c>
-      <c r="F96" t="s">
+      <c r="E96" s="1">
+        <v>180</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97">
+    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
         <v>20220629</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>2209.2779999999998</v>
       </c>
-      <c r="C97">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D97">
+      <c r="C97" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D97" s="1">
         <f t="shared" si="8"/>
         <v>-0.68294919688734879</v>
       </c>
-      <c r="E97">
-        <v>180</v>
-      </c>
-      <c r="F97" t="s">
+      <c r="E97" s="1">
+        <v>180</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98">
+    <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
         <v>20220712</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>2211.98</v>
       </c>
-      <c r="C98">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D98">
+      <c r="C98" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D98" s="1">
         <f t="shared" si="8"/>
         <v>-0.56148206089539454</v>
       </c>
-      <c r="E98">
-        <v>180</v>
-      </c>
-      <c r="F98" t="s">
+      <c r="E98" s="1">
+        <v>180</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99">
+    <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
         <v>20220720</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
         <v>2208.6642099999999</v>
       </c>
-      <c r="C99">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D99">
+      <c r="C99" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D99" s="1">
         <f>100*(B99-C99)/C99</f>
         <v>-0.7105418369319384</v>
       </c>
-      <c r="E99">
-        <v>180</v>
-      </c>
-      <c r="F99" t="s">
+      <c r="E99" s="1">
+        <v>180</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100">
+    <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
         <v>20220722</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="2">
         <v>2217.8699700000002</v>
       </c>
-      <c r="C100">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D100">
+      <c r="C100" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D100" s="1">
         <f>100*(B100-C100)/C100</f>
         <v>-0.29670123669906118</v>
       </c>
-      <c r="E100">
-        <v>180</v>
-      </c>
-      <c r="F100" t="s">
+      <c r="E100" s="1">
+        <v>180</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101">
+    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
         <v>20220722</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="1">
         <v>2217.323202</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="1">
         <f>100*(B101-C101)/C101</f>
         <v>-0.40679479693493792</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="1">
         <v>176</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102">
+    <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
         <v>20220722</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="1">
         <v>2215.267906</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="1">
         <f t="shared" ref="D102" si="9">100*(B102-C102)/C102</f>
         <v>-0.49911039445198346</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="1">
         <v>176</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103">
+    <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
         <v>20220722</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="1">
         <v>2200.7479530000001</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="1">
         <f>D105</f>
         <v>7.1615261163340063E-2</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="1">
         <v>176</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104">
+    <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
         <v>20220723</v>
       </c>
       <c r="B104" s="3">
         <v>2210.2288970017398</v>
       </c>
-      <c r="C104">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D104">
+      <c r="C104" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D104" s="1">
         <f t="shared" ref="D104" si="10">100*(B104-C104)/C104</f>
         <v>-0.64020207052736056</v>
       </c>
-      <c r="E104">
-        <v>180</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="E104" s="1">
+        <v>180</v>
+      </c>
+      <c r="F104" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105">
+    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
         <v>20220729</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="1">
         <v>2226.06306</v>
       </c>
-      <c r="C105">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D105">
+      <c r="C105" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D105" s="1">
         <f t="shared" ref="D105:D130" si="11">100*(B105-C105)/C105</f>
         <v>7.1615261163340063E-2</v>
       </c>
-      <c r="E105">
-        <v>180</v>
-      </c>
-      <c r="F105" t="s">
+      <c r="E105" s="1">
+        <v>180</v>
+      </c>
+      <c r="F105" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106">
+    <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
         <v>20220731</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="1">
         <v>2227.9749999999999</v>
       </c>
-      <c r="C106">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D106">
+      <c r="C106" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D106" s="1">
         <f t="shared" si="11"/>
         <v>0.15756562237297467</v>
       </c>
-      <c r="E106">
-        <v>180</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="E106" s="1">
+        <v>180</v>
+      </c>
+      <c r="F106" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107">
+    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
         <v>20220802</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="1">
         <v>2220.3086600000001</v>
       </c>
-      <c r="C107">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D107">
+      <c r="C107" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D107" s="1">
         <f t="shared" si="11"/>
         <v>-0.18707107760498703</v>
       </c>
-      <c r="E107">
-        <v>180</v>
-      </c>
-      <c r="F107" t="s">
+      <c r="E107" s="1">
+        <v>180</v>
+      </c>
+      <c r="F107" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108">
+    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
         <v>20220805</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="1">
         <v>2219.8236287263899</v>
       </c>
-      <c r="C108">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D108">
+      <c r="C108" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D108" s="1">
         <f t="shared" si="11"/>
         <v>-0.20887542981518878</v>
       </c>
-      <c r="E108">
-        <v>180</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="E108" s="1">
+        <v>180</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109">
+    <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
         <v>20220825</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="1">
         <v>2198.6440400000001</v>
       </c>
-      <c r="C109">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D109">
+      <c r="C109" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D109" s="1">
         <f t="shared" si="11"/>
         <v>-1.16099385471594</v>
       </c>
-      <c r="E109">
-        <v>180</v>
-      </c>
-      <c r="F109" t="s">
+      <c r="E109" s="1">
+        <v>180</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110">
+    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
         <v>20220831</v>
       </c>
-      <c r="B110">
+      <c r="B110" s="1">
         <v>2210.5472799999998</v>
       </c>
-      <c r="C110">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D110">
+      <c r="C110" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D110" s="1">
         <f t="shared" si="11"/>
         <v>-0.62588931295994232</v>
       </c>
-      <c r="E110">
-        <v>180</v>
-      </c>
-      <c r="F110" t="s">
+      <c r="E110" s="1">
+        <v>180</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111">
+    <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
         <v>20220903</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="1">
         <v>2209.65328484982</v>
       </c>
-      <c r="C111">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D111">
+      <c r="C111" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D111" s="1">
         <f t="shared" si="11"/>
         <v>-0.66607844341257871</v>
       </c>
-      <c r="E111">
-        <v>180</v>
-      </c>
-      <c r="F111" t="s">
+      <c r="E111" s="1">
+        <v>180</v>
+      </c>
+      <c r="F111" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112">
+    <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
         <v>20220908</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="1">
         <v>2263.1208099999999</v>
       </c>
-      <c r="C112">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D112">
+      <c r="C112" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D112" s="1">
         <f t="shared" si="11"/>
         <v>1.7375289394777227</v>
       </c>
-      <c r="E112">
-        <v>180</v>
-      </c>
-      <c r="F112" t="s">
+      <c r="E112" s="1">
+        <v>180</v>
+      </c>
+      <c r="F112" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113">
+    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
         <v>20220914</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="1">
         <v>2221.37</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="1">
         <f t="shared" si="11"/>
         <v>-0.22502897079565115</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="1">
         <v>176</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F113" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114">
+    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
         <v>20220916</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="1">
         <v>2193.7814232117898</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="1">
         <f t="shared" si="11"/>
         <v>-1.4641964439228823</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F114" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115">
+    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
         <v>20220916</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="1">
         <v>2194.6040582389001</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="1">
         <f t="shared" si="11"/>
         <v>-1.4272470001122923</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F115" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116">
+    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
         <v>20220930</v>
       </c>
-      <c r="B116">
+      <c r="B116" s="1">
         <v>2219.7338900066802</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="1">
         <f t="shared" si="11"/>
         <v>-0.29851642546734591</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="1">
         <v>176</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F116" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117">
+    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
         <v>20220930</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="1">
         <v>2210.1862615120499</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="1">
         <v>2215.13</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="1">
         <f t="shared" si="11"/>
         <v>-0.22318051256360633</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="1">
         <v>202</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F117" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118">
+    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
         <v>20230118</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="1">
         <v>2276.5568004565698</v>
       </c>
-      <c r="C118">
-        <v>2224.4699999999998</v>
-      </c>
-      <c r="D118">
+      <c r="C118" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D118" s="1">
         <f t="shared" si="11"/>
         <v>2.3415375553084563</v>
       </c>
-      <c r="E118">
-        <v>180</v>
-      </c>
-      <c r="F118" t="s">
+      <c r="E118" s="1">
+        <v>180</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119">
+    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
         <v>20230118</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="1">
         <v>2205.9135813586099</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="1">
         <v>2215.13</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="1">
         <f t="shared" si="11"/>
         <v>-0.41606671578598958</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="1">
         <v>202</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120">
+    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
         <v>20230118</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="1">
         <v>2199.9190495084099</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="1">
         <v>2215.3200000000002</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="1">
         <f t="shared" si="11"/>
         <v>-0.69520206975020604</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="1">
         <v>196</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F120" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121">
+    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
         <v>20230221</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="1">
         <v>2191.1105299999999</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="1">
         <v>2215.3200000000002</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="1">
         <f t="shared" si="11"/>
         <v>-1.0928204503187005</v>
       </c>
-      <c r="E121">
+      <c r="E121" s="1">
         <v>196</v>
       </c>
-      <c r="F121" t="s">
+      <c r="F121" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122">
+    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
         <v>20230412</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="1">
         <v>2206.5646200000001</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="1">
         <v>2215.3200000000002</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="1">
         <f t="shared" si="11"/>
         <v>-0.39521965223985966</v>
       </c>
-      <c r="E122">
+      <c r="E122" s="1">
         <v>196</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F122" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123">
+    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
         <v>20230516</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="1">
         <v>2238.4775300000001</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="1">
         <f t="shared" si="11"/>
         <v>0.54337220061265401</v>
       </c>
-      <c r="E123">
+      <c r="E123" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124">
+      <c r="F123" s="1"/>
+    </row>
+    <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
         <v>20230522</v>
       </c>
-      <c r="B124">
+      <c r="B124" s="1">
         <v>2235.8562700000002</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="1">
         <f t="shared" si="11"/>
         <v>0.42563578544543668</v>
       </c>
-      <c r="E124">
+      <c r="E124" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125">
+      <c r="F124" s="1"/>
+    </row>
+    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
         <v>20230523</v>
       </c>
-      <c r="B125">
+      <c r="B125" s="1">
         <v>2228.1219700000001</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="1">
         <f t="shared" si="11"/>
         <v>7.8242258733910539E-2</v>
       </c>
-      <c r="E125">
+      <c r="E125" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126">
+      <c r="F125" s="1"/>
+    </row>
+    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
         <v>20230525</v>
       </c>
-      <c r="B126">
+      <c r="B126" s="1">
         <v>2231.06837</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="1">
         <f t="shared" si="11"/>
         <v>0.21058264986210123</v>
       </c>
-      <c r="E126">
+      <c r="E126" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127">
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
         <v>20230530</v>
       </c>
-      <c r="B127">
+      <c r="B127" s="1">
         <v>2227.05548</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="1">
         <f t="shared" si="11"/>
         <v>3.0339834170262016E-2</v>
       </c>
-      <c r="E127">
+      <c r="E127" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128">
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
         <v>20230531</v>
       </c>
-      <c r="B128">
+      <c r="B128" s="1">
         <v>2220.5585700000001</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="1">
         <f t="shared" si="11"/>
         <v>-0.26147513003170902</v>
       </c>
-      <c r="E128">
+      <c r="E128" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129">
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
         <v>20230601</v>
       </c>
-      <c r="B129">
+      <c r="B129" s="1">
         <v>2244.2638299999999</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D129">
+      <c r="D129" s="1">
         <f t="shared" si="11"/>
         <v>0.80326943289105013</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130">
+      <c r="F129" s="1"/>
+    </row>
+    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
         <v>20230623</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130" s="2">
         <v>2223.05278</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="1">
         <v>2215.3200000000002</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="1">
         <f t="shared" si="11"/>
         <v>0.34905927811782589</v>
       </c>
-      <c r="E130">
+      <c r="E130" s="1">
         <v>196</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F130" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131">
+    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
         <v>20230713</v>
       </c>
-      <c r="B131">
+      <c r="B131" s="1">
         <v>2217.116</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="1">
         <v>2216.3200000000002</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="1">
         <f t="shared" ref="D131:D137" si="12">100*(B131-C131)/C131</f>
         <v>3.591539127922961E-2</v>
       </c>
-      <c r="E131">
+      <c r="E131" s="1">
         <v>196</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F131" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132">
+    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
         <v>20231103</v>
       </c>
-      <c r="B132">
+      <c r="B132" s="1">
         <v>2229.808</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="1">
         <v>2216.3200000000002</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="1">
         <f t="shared" si="12"/>
         <v>0.60857637886225036</v>
       </c>
-      <c r="E132">
+      <c r="E132" s="1">
         <v>196</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133">
+      <c r="F132" s="1"/>
+    </row>
+    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
         <v>20231110</v>
       </c>
-      <c r="B133" s="4">
+      <c r="B133" s="1">
         <v>2231.6908699999999</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="1">
         <f t="shared" si="12"/>
         <v>0.238542836353174</v>
       </c>
-      <c r="E133">
+      <c r="E133" s="1">
         <v>176</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F133" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A134">
+    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
         <v>20231116</v>
       </c>
-      <c r="B134" s="4">
+      <c r="B134" s="1">
         <v>2235.37547</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="1">
         <v>2226.38</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="1">
         <f t="shared" si="12"/>
         <v>0.40404019080300041</v>
       </c>
-      <c r="E134">
+      <c r="E134" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135">
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
         <v>20240201</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="1">
         <v>2206.982</v>
       </c>
-      <c r="C135">
+      <c r="C135" s="1">
         <v>2215.36</v>
       </c>
-      <c r="D135">
+      <c r="D135" s="1">
         <f t="shared" si="12"/>
         <v>-0.37817781308681914</v>
       </c>
-      <c r="E135">
+      <c r="E135" s="1">
         <v>196</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F135" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136">
+      <c r="A136" s="1">
         <v>20240215</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B136" s="1">
         <v>2230.9595899999999</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="1">
         <v>2215.36</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="1">
         <f t="shared" si="12"/>
         <v>0.70415598367758769</v>
       </c>
-      <c r="E136">
+      <c r="E136" s="1">
         <v>196</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F136" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137">
+      <c r="A137" s="1">
         <v>20240229</v>
       </c>
-      <c r="B137" s="5">
+      <c r="B137" s="1">
         <v>2223.31187</v>
       </c>
-      <c r="C137">
+      <c r="C137" s="1">
         <v>2230.91</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="1">
         <f t="shared" si="12"/>
         <v>-0.34058433554019912</v>
       </c>
-      <c r="E137">
-        <v>180</v>
-      </c>
-      <c r="F137" t="s">
+      <c r="E137" s="1">
+        <v>180</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>20240320</v>
+      </c>
+      <c r="B138" s="1">
+        <v>2215.3408491692098</v>
+      </c>
+      <c r="C138" s="1">
+        <v>2230.91</v>
+      </c>
+      <c r="D138" s="1">
+        <f t="shared" ref="D138" si="13">100*(B138-C138)/C138</f>
+        <v>-0.69788341218561134</v>
+      </c>
+      <c r="E138" s="1">
+        <v>180</v>
+      </c>
+      <c r="F138" s="1" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
calculaated CRM data 0515
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FDED21-A7F6-F54C-A2B9-AA7F3F133B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42E0BB-6DF5-8A49-A440-4EDAD772EFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="500" windowWidth="17900" windowHeight="9520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -1038,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3973,6 +3973,27 @@
         <v>46</v>
       </c>
     </row>
+    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>20240515</v>
+      </c>
+      <c r="B141" s="4">
+        <v>2213.9812200000001</v>
+      </c>
+      <c r="C141" s="1">
+        <v>2209.71801</v>
+      </c>
+      <c r="D141" s="1">
+        <f t="shared" ref="D141" si="16">100*(B141-C141)/C141</f>
+        <v>0.19293004721448923</v>
+      </c>
+      <c r="E141" s="1">
+        <v>180</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding crm and pH data from 6/1/24
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Putnam_Lab/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42E0BB-6DF5-8A49-A440-4EDAD772EFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0119C537-76EC-4351-82E5-97EBE9662266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="500" windowWidth="17900" windowHeight="9520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -174,13 +174,16 @@
   </si>
   <si>
     <t>CRM180_opened20240229_DMB</t>
+  </si>
+  <si>
+    <t>CRM196_opened20240306</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1038,21 +1041,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F141"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C142" sqref="C142"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="J140" sqref="J140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="1">
         <v>20210218</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="1">
         <v>20210221</v>
       </c>
@@ -1114,7 +1117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="1">
         <v>20210228</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="1">
         <v>20210228</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="1">
         <v>20210228</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="1">
         <v>20210228</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="1">
         <v>20210228</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="1">
         <v>20210228</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="1">
         <v>20210228</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="1">
         <v>20210228</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="1">
         <v>20210314</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="1">
         <v>20210314</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="1">
         <v>20210314</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="1">
         <v>20210314</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="1">
         <v>20210314</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75">
       <c r="A17" s="1">
         <v>20210314</v>
       </c>
@@ -1408,7 +1411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.75">
       <c r="A18" s="1">
         <v>20210314</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" s="1">
         <v>20210314</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="1">
         <v>20210314</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="1">
         <v>20210314</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="1">
         <v>20210314</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="1">
         <v>20210314</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15.75">
       <c r="A24" s="1">
         <v>20210328</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15.75">
       <c r="A25" s="1">
         <v>20210328</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15.75">
       <c r="A26" s="1">
         <v>20210328</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="1">
         <v>20210328</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="1">
         <v>20210328</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15.75">
       <c r="A29" s="1">
         <v>20210404</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15.75">
       <c r="A30" s="1">
         <v>20210418</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15.75">
       <c r="A31" s="1">
         <v>20210428</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15.75">
       <c r="A32" s="1">
         <v>20210504</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15.75">
       <c r="A33" s="1">
         <v>20210505</v>
       </c>
@@ -1744,7 +1747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="1">
         <v>20210506</v>
       </c>
@@ -1765,7 +1768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15.75">
       <c r="A35" s="1">
         <v>20210511</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15.75">
       <c r="A36" s="1">
         <v>20210525</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15.75">
       <c r="A37" s="1">
         <v>20210526</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15.75">
       <c r="A38" s="1">
         <v>20210527</v>
       </c>
@@ -1849,7 +1852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15.75">
       <c r="A39" s="1">
         <v>20210601</v>
       </c>
@@ -1870,7 +1873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15.75">
       <c r="A40" s="1">
         <v>20210603</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15.75">
       <c r="A41" s="1">
         <v>20210610</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15.75">
       <c r="A42" s="1">
         <v>20210615</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15.75">
       <c r="A43" s="1">
         <v>20210624</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15.75">
       <c r="A44" s="1">
         <v>20210706</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15.75">
       <c r="A45" s="1">
         <v>20210708</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15.75">
       <c r="A46" s="1">
         <v>20210715</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15.75">
       <c r="A47" s="1">
         <v>20210719</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15.75">
       <c r="A48" s="1">
         <v>20210723</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.75">
       <c r="A49" s="1">
         <v>20210724</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15.75">
       <c r="A50" s="1">
         <v>20210730</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15.75">
       <c r="A51" s="1">
         <v>20210811</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.75">
       <c r="A52" s="1">
         <v>20211018</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75">
       <c r="A53" s="1">
         <v>20211110</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.75">
       <c r="A54" s="1">
         <v>20211117</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15.75">
       <c r="A55" s="1">
         <v>20211206</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15.75">
       <c r="A56" s="1">
         <v>20220118</v>
       </c>
@@ -2227,7 +2230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15.75">
       <c r="A57" s="1">
         <v>20220127</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.75">
       <c r="A58" s="1">
         <v>20220131</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15.75">
       <c r="A59" s="1">
         <v>20220201</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15.75">
       <c r="A60" s="1">
         <v>20220203</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15.75">
       <c r="A61" s="1">
         <v>20220209</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15.75">
       <c r="A62" s="1">
         <v>20220210</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="15.75">
       <c r="A63" s="1">
         <v>20220216</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="15.75">
       <c r="A64" s="1">
         <v>20220224</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15.75">
       <c r="A65" s="1">
         <v>20220302</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15.75">
       <c r="A66" s="1">
         <v>20220303</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15.75">
       <c r="A67" s="1">
         <v>20220308</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="15.75">
       <c r="A68" s="1">
         <v>20220309</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="15.75">
       <c r="A69" s="1">
         <v>20220310</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="15.75">
       <c r="A70" s="1">
         <v>20220311</v>
       </c>
@@ -2521,7 +2524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="15.75">
       <c r="A71" s="1">
         <v>20220314</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="15.75">
       <c r="A72" s="1">
         <v>20220315</v>
       </c>
@@ -2563,7 +2566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="15.75">
       <c r="A73" s="1">
         <v>20220317</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="15.75">
       <c r="A74" s="1">
         <v>20220318</v>
       </c>
@@ -2605,7 +2608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="15.75">
       <c r="A75" s="1">
         <v>20220321</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="15.75">
       <c r="A76" s="1">
         <v>20220322</v>
       </c>
@@ -2647,7 +2650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="15.75">
       <c r="A77" s="1">
         <v>20220323</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="15.75">
       <c r="A78" s="1">
         <v>20220324</v>
       </c>
@@ -2689,7 +2692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15.75">
       <c r="A79" s="1">
         <v>20220329</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="15.75">
       <c r="A80" s="1">
         <v>20220330</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="15.75">
       <c r="A81" s="1">
         <v>20220331</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="15.75">
       <c r="A82" s="1">
         <v>20220401</v>
       </c>
@@ -2773,7 +2776,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="15.75">
       <c r="A83" s="1">
         <v>20220404</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="15.75">
       <c r="A84" s="1">
         <v>20220405</v>
       </c>
@@ -2815,7 +2818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="15.75">
       <c r="A85" s="1">
         <v>20220406</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="15.75">
       <c r="A86" s="1">
         <v>20220407</v>
       </c>
@@ -2857,7 +2860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="15.75">
       <c r="A87" s="1">
         <v>20220408</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="15.75">
       <c r="A88" s="1">
         <v>20220413</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="15.75">
       <c r="A89" s="1">
         <v>20220415</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="15.75">
       <c r="A90" s="1">
         <v>20220420</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="15.75">
       <c r="A91" s="1">
         <v>20220427</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="15.75">
       <c r="A92" s="1">
         <v>20220504</v>
       </c>
@@ -2983,7 +2986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="15.75">
       <c r="A93" s="1">
         <v>20220518</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="15.75">
       <c r="A94" s="1">
         <v>20220520</v>
       </c>
@@ -3025,7 +3028,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="15.75">
       <c r="A95" s="1">
         <v>20220608</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="15.75">
       <c r="A96" s="1">
         <v>20220621</v>
       </c>
@@ -3067,7 +3070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="15.75">
       <c r="A97" s="1">
         <v>20220629</v>
       </c>
@@ -3088,7 +3091,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="15.75">
       <c r="A98" s="1">
         <v>20220712</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="15.75">
       <c r="A99" s="1">
         <v>20220720</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="15.75">
       <c r="A100" s="1">
         <v>20220722</v>
       </c>
@@ -3151,7 +3154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="15.75">
       <c r="A101" s="1">
         <v>20220722</v>
       </c>
@@ -3172,7 +3175,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="15.75">
       <c r="A102" s="1">
         <v>20220722</v>
       </c>
@@ -3193,7 +3196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="15.75">
       <c r="A103" s="1">
         <v>20220722</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="15.75">
       <c r="A104" s="1">
         <v>20220723</v>
       </c>
@@ -3235,7 +3238,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="15.75">
       <c r="A105" s="1">
         <v>20220729</v>
       </c>
@@ -3256,7 +3259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="15.75">
       <c r="A106" s="1">
         <v>20220731</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="15.75">
       <c r="A107" s="1">
         <v>20220802</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" ht="15.75">
       <c r="A108" s="1">
         <v>20220805</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" ht="15.75">
       <c r="A109" s="1">
         <v>20220825</v>
       </c>
@@ -3340,7 +3343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" ht="15.75">
       <c r="A110" s="1">
         <v>20220831</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" ht="15.75">
       <c r="A111" s="1">
         <v>20220903</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" ht="15.75">
       <c r="A112" s="1">
         <v>20220908</v>
       </c>
@@ -3403,7 +3406,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" ht="15.75">
       <c r="A113" s="1">
         <v>20220914</v>
       </c>
@@ -3424,7 +3427,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="15.75">
       <c r="A114" s="1">
         <v>20220916</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" ht="15.75">
       <c r="A115" s="1">
         <v>20220916</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" ht="15.75">
       <c r="A116" s="1">
         <v>20220930</v>
       </c>
@@ -3487,7 +3490,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="15.75">
       <c r="A117" s="1">
         <v>20220930</v>
       </c>
@@ -3508,7 +3511,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" ht="15.75">
       <c r="A118" s="1">
         <v>20230118</v>
       </c>
@@ -3529,7 +3532,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" ht="15.75">
       <c r="A119" s="1">
         <v>20230118</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="15.75">
       <c r="A120" s="1">
         <v>20230118</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="15.75">
       <c r="A121" s="1">
         <v>20230221</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" ht="15.75">
       <c r="A122" s="1">
         <v>20230412</v>
       </c>
@@ -3613,7 +3616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="15.75">
       <c r="A123" s="1">
         <v>20230516</v>
       </c>
@@ -3632,7 +3635,7 @@
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="15.75">
       <c r="A124" s="1">
         <v>20230522</v>
       </c>
@@ -3651,7 +3654,7 @@
       </c>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="15.75">
       <c r="A125" s="1">
         <v>20230523</v>
       </c>
@@ -3670,7 +3673,7 @@
       </c>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="15.75">
       <c r="A126" s="1">
         <v>20230525</v>
       </c>
@@ -3689,7 +3692,7 @@
       </c>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="15.75">
       <c r="A127" s="1">
         <v>20230530</v>
       </c>
@@ -3708,7 +3711,7 @@
       </c>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="15.75">
       <c r="A128" s="1">
         <v>20230531</v>
       </c>
@@ -3727,7 +3730,7 @@
       </c>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="15.75">
       <c r="A129" s="1">
         <v>20230601</v>
       </c>
@@ -3746,7 +3749,7 @@
       </c>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="15.75">
       <c r="A130" s="1">
         <v>20230623</v>
       </c>
@@ -3767,7 +3770,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="15.75">
       <c r="A131" s="1">
         <v>20230713</v>
       </c>
@@ -3788,7 +3791,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="15.75">
       <c r="A132" s="1">
         <v>20231103</v>
       </c>
@@ -3807,7 +3810,7 @@
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="15.75">
       <c r="A133" s="1">
         <v>20231110</v>
       </c>
@@ -3828,7 +3831,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="15.75">
       <c r="A134" s="1">
         <v>20231116</v>
       </c>
@@ -3847,7 +3850,7 @@
       </c>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="15.75">
       <c r="A135" s="1">
         <v>20240201</v>
       </c>
@@ -3868,7 +3871,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="15.75">
       <c r="A136" s="1">
         <v>20240215</v>
       </c>
@@ -3889,7 +3892,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="15.75">
       <c r="A137" s="1">
         <v>20240229</v>
       </c>
@@ -3910,7 +3913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="15.75">
       <c r="A138" s="1">
         <v>20240320</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="15.75">
       <c r="A139" s="1">
         <v>20240404</v>
       </c>
@@ -3952,7 +3955,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="15.75">
       <c r="A140" s="1">
         <v>20240430</v>
       </c>
@@ -3973,7 +3976,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="15.75">
       <c r="A141" s="1">
         <v>20240515</v>
       </c>
@@ -3992,6 +3995,17 @@
       </c>
       <c r="F141" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="15.75">
+      <c r="A142" s="1">
+        <v>20240601</v>
+      </c>
+      <c r="E142" s="1">
+        <v>196</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dmb training titrations sarah and eliza
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPP Lab\Documents\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0119C537-76EC-4351-82E5-97EBE9662266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63394AE-DDFA-443B-802A-05FC7DCC240C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="735" windowWidth="16635" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -1043,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="J140" sqref="J140"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3858,11 +3858,11 @@
         <v>2206.982</v>
       </c>
       <c r="C135" s="1">
-        <v>2215.36</v>
+        <v>2215.3200000000002</v>
       </c>
       <c r="D135" s="1">
         <f t="shared" si="12"/>
-        <v>-0.37817781308681914</v>
+        <v>-0.37637903327736816</v>
       </c>
       <c r="E135" s="1">
         <v>196</v>
@@ -3879,11 +3879,11 @@
         <v>2230.9595899999999</v>
       </c>
       <c r="C136" s="1">
-        <v>2215.36</v>
+        <v>2215.3200000000002</v>
       </c>
       <c r="D136" s="1">
         <f t="shared" si="12"/>
-        <v>0.70415598367758769</v>
+        <v>0.70597430619503143</v>
       </c>
       <c r="E136" s="1">
         <v>196</v>
@@ -3900,11 +3900,11 @@
         <v>2223.31187</v>
       </c>
       <c r="C137" s="1">
-        <v>2230.91</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D137" s="1">
         <f t="shared" si="12"/>
-        <v>-0.34058433554019912</v>
+        <v>-5.2063188085242823E-2</v>
       </c>
       <c r="E137" s="1">
         <v>180</v>
@@ -3921,11 +3921,11 @@
         <v>2215.3408491692098</v>
       </c>
       <c r="C138" s="1">
-        <v>2230.91</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D138" s="1">
         <f t="shared" ref="D138" si="13">100*(B138-C138)/C138</f>
-        <v>-0.69788341218561134</v>
+        <v>-0.41039667115267764</v>
       </c>
       <c r="E138" s="1">
         <v>180</v>
@@ -3942,11 +3942,11 @@
         <v>2218.2933899999998</v>
       </c>
       <c r="C139" s="1">
-        <v>2230.91</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D139" s="1">
         <f t="shared" ref="D139" si="14">100*(B139-C139)/C139</f>
-        <v>-0.56553648511145849</v>
+        <v>-0.27766659024396745</v>
       </c>
       <c r="E139" s="1">
         <v>180</v>
@@ -3963,11 +3963,11 @@
         <v>2213.9812200000001</v>
       </c>
       <c r="C140" s="1">
-        <v>2230.91</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D140" s="1">
-        <f t="shared" ref="D140" si="15">100*(B140-C140)/C140</f>
-        <v>-0.75882846013508987</v>
+        <f t="shared" ref="D140:D141" si="15">100*(B140-C140)/C140</f>
+        <v>-0.47151815938177094</v>
       </c>
       <c r="E140" s="1">
         <v>180</v>
@@ -3980,15 +3980,15 @@
       <c r="A141" s="1">
         <v>20240515</v>
       </c>
-      <c r="B141" s="4">
-        <v>2213.9812200000001</v>
+      <c r="B141" s="1">
+        <v>2209.71801</v>
       </c>
       <c r="C141" s="1">
-        <v>2209.71801</v>
+        <v>2224.4699999999998</v>
       </c>
       <c r="D141" s="1">
-        <f t="shared" ref="D141" si="16">100*(B141-C141)/C141</f>
-        <v>0.19293004721448923</v>
+        <f t="shared" si="15"/>
+        <v>-0.6631687548045041</v>
       </c>
       <c r="E141" s="1">
         <v>180</v>
@@ -4000,6 +4000,16 @@
     <row r="142" spans="1:6" ht="15.75">
       <c r="A142" s="1">
         <v>20240601</v>
+      </c>
+      <c r="B142" s="1">
+        <v>2202.70937</v>
+      </c>
+      <c r="C142" s="1">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D142" s="1">
+        <f t="shared" ref="D141:D142" si="16">100*(B142-C142)/C142</f>
+        <v>-0.56924642940975245</v>
       </c>
       <c r="E142" s="1">
         <v>196</v>

</xml_diff>

<commit_message>
added crm for 20240613
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5799228-9FC3-7B46-850D-779FF8E89A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D284BF3-2A6F-9A45-91C3-B242C29DB7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="740" windowWidth="21560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="660" windowWidth="21560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>CRM196_opened20240306</t>
+  </si>
+  <si>
+    <t>CRM196_opened20240613</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="G144" sqref="G144"/>
+      <selection activeCell="J143" sqref="J143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4016,7 +4019,7 @@
         <v>2215.3200000000002</v>
       </c>
       <c r="D142" s="1">
-        <f t="shared" ref="D142:D143" si="16">100*(B142-C142)/C142</f>
+        <f t="shared" ref="D142:D144" si="16">100*(B142-C142)/C142</f>
         <v>-0.56924642940975245</v>
       </c>
       <c r="E142" s="1">
@@ -4045,6 +4048,27 @@
       </c>
       <c r="F143" s="1" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>20240613</v>
+      </c>
+      <c r="B144" s="1">
+        <v>2207.7169100000001</v>
+      </c>
+      <c r="C144" s="1">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D144" s="1">
+        <f t="shared" si="16"/>
+        <v>-0.3432050448693672</v>
+      </c>
+      <c r="E144" s="1">
+        <v>196</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated CRM data for titrations
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D284BF3-2A6F-9A45-91C3-B242C29DB7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18352B00-E0E1-CD46-BA42-099341979886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="660" windowWidth="21560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="50">
   <si>
     <t>Date</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>CRM196_opened20240613</t>
+  </si>
+  <si>
+    <t>CRM196_opened20240614</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="J143" sqref="J143"/>
+      <selection activeCell="F138" sqref="F138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4071,6 +4074,27 @@
         <v>48</v>
       </c>
     </row>
+    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>20240711</v>
+      </c>
+      <c r="B145" s="1">
+        <v>2215.1301800000001</v>
+      </c>
+      <c r="C145" s="1">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D145" s="1">
+        <f t="shared" ref="D145" si="17">100*(B145-C145)/C145</f>
+        <v>-8.568513803877284E-3</v>
+      </c>
+      <c r="E145" s="1">
+        <v>196</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding QT TA data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Danielle/Desktop/Titrator/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uri0-my.sharepoint.com/personal/ffields_uri_edu/Documents/GitHub/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61F169E-2240-2243-AE7C-5EB0645B3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{E61F169E-2240-2243-AE7C-5EB0645B3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D3A85D1-B863-42BB-9FA2-9C2DA1E2E9DF}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="660" windowWidth="21560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -183,13 +183,25 @@
   </si>
   <si>
     <t>CRM196_opened20240614</t>
+  </si>
+  <si>
+    <t>CRM196_opened20240828</t>
+  </si>
+  <si>
+    <t>Issue with titration, complete values were not recorded in file</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CRM196_opened20240829</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1055,21 +1067,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B150" sqref="B150:B151"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1328125" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="1">
         <v>20210218</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15.75">
       <c r="A3" s="1">
         <v>20210221</v>
       </c>
@@ -1131,7 +1143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15.75">
       <c r="A4" s="1">
         <v>20210228</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="1">
         <v>20210228</v>
       </c>
@@ -1173,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15.75">
       <c r="A6" s="1">
         <v>20210228</v>
       </c>
@@ -1194,7 +1206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="1">
         <v>20210228</v>
       </c>
@@ -1215,7 +1227,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.75">
       <c r="A8" s="1">
         <v>20210228</v>
       </c>
@@ -1236,7 +1248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.75">
       <c r="A9" s="1">
         <v>20210228</v>
       </c>
@@ -1257,7 +1269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15.75">
       <c r="A10" s="1">
         <v>20210228</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15.75">
       <c r="A11" s="1">
         <v>20210228</v>
       </c>
@@ -1299,7 +1311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15.75">
       <c r="A12" s="1">
         <v>20210314</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.75">
       <c r="A13" s="1">
         <v>20210314</v>
       </c>
@@ -1341,7 +1353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.75">
       <c r="A14" s="1">
         <v>20210314</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.75">
       <c r="A15" s="1">
         <v>20210314</v>
       </c>
@@ -1383,7 +1395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.75">
       <c r="A16" s="1">
         <v>20210314</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15.75">
       <c r="A17" s="1">
         <v>20210314</v>
       </c>
@@ -1425,7 +1437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15.75">
       <c r="A18" s="1">
         <v>20210314</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" s="1">
         <v>20210314</v>
       </c>
@@ -1467,7 +1479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="1">
         <v>20210314</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="1">
         <v>20210314</v>
       </c>
@@ -1509,7 +1521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="1">
         <v>20210314</v>
       </c>
@@ -1530,7 +1542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="1">
         <v>20210314</v>
       </c>
@@ -1551,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15.75">
       <c r="A24" s="1">
         <v>20210328</v>
       </c>
@@ -1572,7 +1584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15.75">
       <c r="A25" s="1">
         <v>20210328</v>
       </c>
@@ -1593,7 +1605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15.75">
       <c r="A26" s="1">
         <v>20210328</v>
       </c>
@@ -1614,7 +1626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="1">
         <v>20210328</v>
       </c>
@@ -1635,7 +1647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="1">
         <v>20210328</v>
       </c>
@@ -1656,7 +1668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15.75">
       <c r="A29" s="1">
         <v>20210404</v>
       </c>
@@ -1677,7 +1689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15.75">
       <c r="A30" s="1">
         <v>20210418</v>
       </c>
@@ -1698,7 +1710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15.75">
       <c r="A31" s="1">
         <v>20210428</v>
       </c>
@@ -1719,7 +1731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15.75">
       <c r="A32" s="1">
         <v>20210504</v>
       </c>
@@ -1740,7 +1752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15.75">
       <c r="A33" s="1">
         <v>20210505</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15.75">
       <c r="A34" s="1">
         <v>20210506</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15.75">
       <c r="A35" s="1">
         <v>20210511</v>
       </c>
@@ -1803,7 +1815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15.75">
       <c r="A36" s="1">
         <v>20210525</v>
       </c>
@@ -1824,7 +1836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15.75">
       <c r="A37" s="1">
         <v>20210526</v>
       </c>
@@ -1845,7 +1857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15.75">
       <c r="A38" s="1">
         <v>20210527</v>
       </c>
@@ -1866,7 +1878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15.75">
       <c r="A39" s="1">
         <v>20210601</v>
       </c>
@@ -1887,7 +1899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15.75">
       <c r="A40" s="1">
         <v>20210603</v>
       </c>
@@ -1908,7 +1920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15.75">
       <c r="A41" s="1">
         <v>20210610</v>
       </c>
@@ -1929,7 +1941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15.75">
       <c r="A42" s="1">
         <v>20210615</v>
       </c>
@@ -1950,7 +1962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15.75">
       <c r="A43" s="1">
         <v>20210624</v>
       </c>
@@ -1971,7 +1983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15.75">
       <c r="A44" s="1">
         <v>20210706</v>
       </c>
@@ -1992,7 +2004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15.75">
       <c r="A45" s="1">
         <v>20210708</v>
       </c>
@@ -2013,7 +2025,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15.75">
       <c r="A46" s="1">
         <v>20210715</v>
       </c>
@@ -2034,7 +2046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15.75">
       <c r="A47" s="1">
         <v>20210719</v>
       </c>
@@ -2055,7 +2067,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15.75">
       <c r="A48" s="1">
         <v>20210723</v>
       </c>
@@ -2076,7 +2088,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.75">
       <c r="A49" s="1">
         <v>20210724</v>
       </c>
@@ -2097,7 +2109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15.75">
       <c r="A50" s="1">
         <v>20210730</v>
       </c>
@@ -2118,7 +2130,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15.75">
       <c r="A51" s="1">
         <v>20210811</v>
       </c>
@@ -2139,7 +2151,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.75">
       <c r="A52" s="1">
         <v>20211018</v>
       </c>
@@ -2160,7 +2172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75">
       <c r="A53" s="1">
         <v>20211110</v>
       </c>
@@ -2181,7 +2193,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.75">
       <c r="A54" s="1">
         <v>20211117</v>
       </c>
@@ -2202,7 +2214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15.75">
       <c r="A55" s="1">
         <v>20211206</v>
       </c>
@@ -2223,7 +2235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15.75">
       <c r="A56" s="1">
         <v>20220118</v>
       </c>
@@ -2244,7 +2256,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15.75">
       <c r="A57" s="1">
         <v>20220127</v>
       </c>
@@ -2265,7 +2277,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.75">
       <c r="A58" s="1">
         <v>20220131</v>
       </c>
@@ -2286,7 +2298,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15.75">
       <c r="A59" s="1">
         <v>20220201</v>
       </c>
@@ -2307,7 +2319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15.75">
       <c r="A60" s="1">
         <v>20220203</v>
       </c>
@@ -2328,7 +2340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15.75">
       <c r="A61" s="1">
         <v>20220209</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15.75">
       <c r="A62" s="1">
         <v>20220210</v>
       </c>
@@ -2370,7 +2382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="15.75">
       <c r="A63" s="1">
         <v>20220216</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="15.75">
       <c r="A64" s="1">
         <v>20220224</v>
       </c>
@@ -2412,7 +2424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15.75">
       <c r="A65" s="1">
         <v>20220302</v>
       </c>
@@ -2433,7 +2445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15.75">
       <c r="A66" s="1">
         <v>20220303</v>
       </c>
@@ -2454,7 +2466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15.75">
       <c r="A67" s="1">
         <v>20220308</v>
       </c>
@@ -2475,7 +2487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="15.75">
       <c r="A68" s="1">
         <v>20220309</v>
       </c>
@@ -2496,7 +2508,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="15.75">
       <c r="A69" s="1">
         <v>20220310</v>
       </c>
@@ -2517,7 +2529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="15.75">
       <c r="A70" s="1">
         <v>20220311</v>
       </c>
@@ -2538,7 +2550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="15.75">
       <c r="A71" s="1">
         <v>20220314</v>
       </c>
@@ -2559,7 +2571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="15.75">
       <c r="A72" s="1">
         <v>20220315</v>
       </c>
@@ -2580,7 +2592,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="15.75">
       <c r="A73" s="1">
         <v>20220317</v>
       </c>
@@ -2601,7 +2613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="15.75">
       <c r="A74" s="1">
         <v>20220318</v>
       </c>
@@ -2622,7 +2634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="15.75">
       <c r="A75" s="1">
         <v>20220321</v>
       </c>
@@ -2643,7 +2655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="15.75">
       <c r="A76" s="1">
         <v>20220322</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="15.75">
       <c r="A77" s="1">
         <v>20220323</v>
       </c>
@@ -2685,7 +2697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="15.75">
       <c r="A78" s="1">
         <v>20220324</v>
       </c>
@@ -2706,7 +2718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15.75">
       <c r="A79" s="1">
         <v>20220329</v>
       </c>
@@ -2727,7 +2739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="15.75">
       <c r="A80" s="1">
         <v>20220330</v>
       </c>
@@ -2748,7 +2760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="15.75">
       <c r="A81" s="1">
         <v>20220331</v>
       </c>
@@ -2769,7 +2781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="15.75">
       <c r="A82" s="1">
         <v>20220401</v>
       </c>
@@ -2790,7 +2802,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" ht="15.75">
       <c r="A83" s="1">
         <v>20220404</v>
       </c>
@@ -2811,7 +2823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="15.75">
       <c r="A84" s="1">
         <v>20220405</v>
       </c>
@@ -2832,7 +2844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="15.75">
       <c r="A85" s="1">
         <v>20220406</v>
       </c>
@@ -2853,7 +2865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="15.75">
       <c r="A86" s="1">
         <v>20220407</v>
       </c>
@@ -2874,7 +2886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="15.75">
       <c r="A87" s="1">
         <v>20220408</v>
       </c>
@@ -2895,7 +2907,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="15.75">
       <c r="A88" s="1">
         <v>20220413</v>
       </c>
@@ -2916,7 +2928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="15.75">
       <c r="A89" s="1">
         <v>20220415</v>
       </c>
@@ -2937,7 +2949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="15.75">
       <c r="A90" s="1">
         <v>20220420</v>
       </c>
@@ -2958,7 +2970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="15.75">
       <c r="A91" s="1">
         <v>20220427</v>
       </c>
@@ -2979,7 +2991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="15.75">
       <c r="A92" s="1">
         <v>20220504</v>
       </c>
@@ -3000,7 +3012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="15.75">
       <c r="A93" s="1">
         <v>20220518</v>
       </c>
@@ -3021,7 +3033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="15.75">
       <c r="A94" s="1">
         <v>20220520</v>
       </c>
@@ -3042,7 +3054,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="15.75">
       <c r="A95" s="1">
         <v>20220608</v>
       </c>
@@ -3063,7 +3075,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="15.75">
       <c r="A96" s="1">
         <v>20220621</v>
       </c>
@@ -3084,7 +3096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="15.75">
       <c r="A97" s="1">
         <v>20220629</v>
       </c>
@@ -3105,7 +3117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="15.75">
       <c r="A98" s="1">
         <v>20220712</v>
       </c>
@@ -3126,7 +3138,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="15.75">
       <c r="A99" s="1">
         <v>20220720</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="15.75">
       <c r="A100" s="1">
         <v>20220722</v>
       </c>
@@ -3168,7 +3180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="15.75">
       <c r="A101" s="1">
         <v>20220722</v>
       </c>
@@ -3189,7 +3201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="15.75">
       <c r="A102" s="1">
         <v>20220722</v>
       </c>
@@ -3210,7 +3222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="15.75">
       <c r="A103" s="1">
         <v>20220722</v>
       </c>
@@ -3231,7 +3243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="15.75">
       <c r="A104" s="1">
         <v>20220723</v>
       </c>
@@ -3252,7 +3264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="15.75">
       <c r="A105" s="1">
         <v>20220729</v>
       </c>
@@ -3273,7 +3285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="15.75">
       <c r="A106" s="1">
         <v>20220731</v>
       </c>
@@ -3294,7 +3306,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="15.75">
       <c r="A107" s="1">
         <v>20220802</v>
       </c>
@@ -3315,7 +3327,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" ht="15.75">
       <c r="A108" s="1">
         <v>20220805</v>
       </c>
@@ -3336,7 +3348,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" ht="15.75">
       <c r="A109" s="1">
         <v>20220825</v>
       </c>
@@ -3357,7 +3369,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" ht="15.75">
       <c r="A110" s="1">
         <v>20220831</v>
       </c>
@@ -3378,7 +3390,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" ht="15.75">
       <c r="A111" s="1">
         <v>20220903</v>
       </c>
@@ -3399,7 +3411,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" ht="15.75">
       <c r="A112" s="1">
         <v>20220908</v>
       </c>
@@ -3420,7 +3432,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" ht="15.75">
       <c r="A113" s="1">
         <v>20220914</v>
       </c>
@@ -3441,7 +3453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="15.75">
       <c r="A114" s="1">
         <v>20220916</v>
       </c>
@@ -3462,7 +3474,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" ht="15.75">
       <c r="A115" s="1">
         <v>20220916</v>
       </c>
@@ -3483,7 +3495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" ht="15.75">
       <c r="A116" s="1">
         <v>20220930</v>
       </c>
@@ -3504,7 +3516,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" ht="15.75">
       <c r="A117" s="1">
         <v>20220930</v>
       </c>
@@ -3525,7 +3537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" ht="15.75">
       <c r="A118" s="1">
         <v>20230118</v>
       </c>
@@ -3546,7 +3558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" ht="15.75">
       <c r="A119" s="1">
         <v>20230118</v>
       </c>
@@ -3567,7 +3579,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" ht="15.75">
       <c r="A120" s="1">
         <v>20230118</v>
       </c>
@@ -3588,7 +3600,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" ht="15.75">
       <c r="A121" s="1">
         <v>20230221</v>
       </c>
@@ -3609,7 +3621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" ht="15.75">
       <c r="A122" s="1">
         <v>20230412</v>
       </c>
@@ -3630,7 +3642,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" ht="15.75">
       <c r="A123" s="1">
         <v>20230516</v>
       </c>
@@ -3649,7 +3661,7 @@
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" ht="15.75">
       <c r="A124" s="1">
         <v>20230522</v>
       </c>
@@ -3668,7 +3680,7 @@
       </c>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" ht="15.75">
       <c r="A125" s="1">
         <v>20230523</v>
       </c>
@@ -3687,7 +3699,7 @@
       </c>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" ht="15.75">
       <c r="A126" s="1">
         <v>20230525</v>
       </c>
@@ -3706,7 +3718,7 @@
       </c>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" ht="15.75">
       <c r="A127" s="1">
         <v>20230530</v>
       </c>
@@ -3725,7 +3737,7 @@
       </c>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" ht="15.75">
       <c r="A128" s="1">
         <v>20230531</v>
       </c>
@@ -3744,7 +3756,7 @@
       </c>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="15.75">
       <c r="A129" s="1">
         <v>20230601</v>
       </c>
@@ -3763,7 +3775,7 @@
       </c>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="15.75">
       <c r="A130" s="1">
         <v>20230623</v>
       </c>
@@ -3784,7 +3796,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="15.75">
       <c r="A131" s="1">
         <v>20230713</v>
       </c>
@@ -3805,7 +3817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="15.75">
       <c r="A132" s="1">
         <v>20231103</v>
       </c>
@@ -3824,7 +3836,7 @@
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="15.75">
       <c r="A133" s="1">
         <v>20231110</v>
       </c>
@@ -3845,7 +3857,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="15.75">
       <c r="A134" s="1">
         <v>20231116</v>
       </c>
@@ -3864,7 +3876,7 @@
       </c>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="15.75">
       <c r="A135" s="1">
         <v>20240201</v>
       </c>
@@ -3885,7 +3897,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="15.75">
       <c r="A136" s="1">
         <v>20240215</v>
       </c>
@@ -3906,7 +3918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="15.75">
       <c r="A137" s="1">
         <v>20240229</v>
       </c>
@@ -3927,7 +3939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="15.75">
       <c r="A138" s="1">
         <v>20240320</v>
       </c>
@@ -3948,7 +3960,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="15.75">
       <c r="A139" s="1">
         <v>20240404</v>
       </c>
@@ -3969,7 +3981,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="15.75">
       <c r="A140" s="1">
         <v>20240430</v>
       </c>
@@ -3990,7 +4002,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="15.75">
       <c r="A141" s="1">
         <v>20240515</v>
       </c>
@@ -4011,7 +4023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" ht="15.75">
       <c r="A142" s="1">
         <v>20240601</v>
       </c>
@@ -4032,7 +4044,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" ht="15.75">
       <c r="A143" s="1">
         <v>20240604</v>
       </c>
@@ -4053,7 +4065,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" ht="15.75">
       <c r="A144" s="1">
         <v>20240613</v>
       </c>
@@ -4074,7 +4086,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" ht="15.75">
       <c r="A145" s="1">
         <v>20240711</v>
       </c>
@@ -4095,7 +4107,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" ht="15.75">
       <c r="A146" s="1">
         <v>20240725</v>
       </c>
@@ -4116,7 +4128,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" ht="15.75">
       <c r="A147" s="1">
         <v>20240806</v>
       </c>
@@ -4135,6 +4147,43 @@
       </c>
       <c r="F147" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="15.75">
+      <c r="A148" s="1">
+        <v>20240924</v>
+      </c>
+      <c r="B148" t="s">
+        <v>52</v>
+      </c>
+      <c r="C148" s="1">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D148" t="s">
+        <v>52</v>
+      </c>
+      <c r="E148" s="1">
+        <v>196</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G148" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="15.75">
+      <c r="A149" s="1">
+        <v>20240924</v>
+      </c>
+      <c r="C149" s="1">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="E149" s="1">
+        <v>196</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding crm data from R
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uri0-my.sharepoint.com/personal/ffields_uri_edu/Documents/GitHub/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{E61F169E-2240-2243-AE7C-5EB0645B3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D3A85D1-B863-42BB-9FA2-9C2DA1E2E9DF}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{E61F169E-2240-2243-AE7C-5EB0645B3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA39692-00EB-4A2F-A434-6B60F3F186C2}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>CRM196_opened20240829</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -4139,7 +4142,7 @@
         <v>2215.3200000000002</v>
       </c>
       <c r="D147" s="1">
-        <f t="shared" ref="D147" si="19">100*(B147-C147)/C147</f>
+        <f t="shared" ref="D147:D149" si="19">100*(B147-C147)/C147</f>
         <v>0.18398876911686429</v>
       </c>
       <c r="E147" s="1">
@@ -4159,8 +4162,8 @@
       <c r="C148" s="1">
         <v>2215.3200000000002</v>
       </c>
-      <c r="D148" t="s">
-        <v>52</v>
+      <c r="D148" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E148" s="1">
         <v>196</v>
@@ -4176,8 +4179,15 @@
       <c r="A149" s="1">
         <v>20240924</v>
       </c>
+      <c r="B149" s="5">
+        <v>2215.33356580073</v>
+      </c>
       <c r="C149" s="1">
         <v>2215.3200000000002</v>
+      </c>
+      <c r="D149" s="1">
+        <f t="shared" si="19"/>
+        <v>6.12363032419398E-4</v>
       </c>
       <c r="E149" s="1">
         <v>196</v>

</xml_diff>

<commit_message>
adding crm accuracy data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uri0-my.sharepoint.com/personal/ffields_uri_edu/Documents/GitHub/Putnam_Lab/Titrator/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{E61F169E-2240-2243-AE7C-5EB0645B3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FA39692-00EB-4A2F-A434-6B60F3F186C2}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{E61F169E-2240-2243-AE7C-5EB0645B3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{612AB7FB-ED09-499A-84B2-CF729400A90A}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -189,12 +189,6 @@
   </si>
   <si>
     <t>Issue with titration, complete values were not recorded in file</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>CRM196_opened20240829</t>
   </si>
   <si>
     <t>n/a</t>
@@ -1070,7 +1064,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
       <selection activeCell="B149" sqref="B149"/>
@@ -1079,7 +1073,7 @@
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1328125" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="6" max="6" width="21.796875" customWidth="1"/>
   </cols>
@@ -4142,7 +4136,7 @@
         <v>2215.3200000000002</v>
       </c>
       <c r="D147" s="1">
-        <f t="shared" ref="D147:D149" si="19">100*(B147-C147)/C147</f>
+        <f t="shared" ref="D147:D150" si="19">100*(B147-C147)/C147</f>
         <v>0.18398876911686429</v>
       </c>
       <c r="E147" s="1">
@@ -4163,7 +4157,7 @@
         <v>2215.3200000000002</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E148" s="1">
         <v>196</v>
@@ -4193,7 +4187,28 @@
         <v>196</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="15.75">
+      <c r="A150" s="1">
+        <v>20241001</v>
+      </c>
+      <c r="B150">
+        <v>2207.22277248604</v>
+      </c>
+      <c r="C150" s="1">
+        <v>2215.3200000000002</v>
+      </c>
+      <c r="D150" s="1">
+        <f t="shared" si="19"/>
+        <v>-0.36551051378402244</v>
+      </c>
+      <c r="E150" s="1">
+        <v>196</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRM Accuracy Data and pH plot
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swimg\OneDrive\Desktop\Putnam-Lab\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF273DA-4072-4CE5-80D8-F0089217879B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3E21C3-71C7-4471-BF69-9543B41F6CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRMAccuracyData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -1082,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4393,7 +4393,25 @@
       </c>
     </row>
     <row r="159" spans="1:6" ht="15.75">
-      <c r="D159" s="1"/>
+      <c r="A159" s="1">
+        <v>20250214</v>
+      </c>
+      <c r="B159">
+        <v>2198.30305</v>
+      </c>
+      <c r="C159" s="1">
+        <v>2215.13</v>
+      </c>
+      <c r="D159" s="1">
+        <f t="shared" ref="D159" si="19">100*(B159-C159)/C159</f>
+        <v>-0.75963713190648507</v>
+      </c>
+      <c r="E159" s="1">
+        <v>202</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="160" spans="1:6" ht="15.75">
       <c r="D160" s="1"/>

</xml_diff>

<commit_message>
Titration data for 0714
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PUTNAM LAB\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C7D91D-1576-49FB-A2EF-70D3A101CBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55490546-8EDE-41B5-AB49-6B74D1BDE6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>CRM180_opened20250502_SS</t>
+  </si>
+  <si>
+    <t>CRM180_opened20250714_PP</t>
   </si>
 </sst>
 </file>
@@ -1073,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="I163" sqref="I163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4459,7 +4462,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D162" s="1">
-        <f t="shared" ref="D162:D164" si="20">100*(B162-C162)/C162</f>
+        <f t="shared" ref="D162:D167" si="20">100*(B162-C162)/C162</f>
         <v>-2.1396062085382019</v>
       </c>
       <c r="E162" s="1">
@@ -4509,6 +4512,69 @@
       </c>
       <c r="F164" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" ht="15.6">
+      <c r="A165" s="5">
+        <v>20250714</v>
+      </c>
+      <c r="B165" s="5">
+        <v>2216.045439</v>
+      </c>
+      <c r="C165" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D165" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.37872216752753751</v>
+      </c>
+      <c r="E165" s="1">
+        <v>180</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="15.6">
+      <c r="A166" s="5">
+        <v>20250714</v>
+      </c>
+      <c r="B166" s="5">
+        <v>2216.900314</v>
+      </c>
+      <c r="C166" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D166" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.34029166498086377</v>
+      </c>
+      <c r="E166" s="1">
+        <v>180</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" ht="15.6">
+      <c r="A167" s="5">
+        <v>20250714</v>
+      </c>
+      <c r="B167" s="5">
+        <v>2220.3447169999999</v>
+      </c>
+      <c r="C167" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D167" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.18545015217107241</v>
+      </c>
+      <c r="E167" s="1">
+        <v>180</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
crm plots and data
</commit_message>
<xml_diff>
--- a/Data/CRMAccuracyData.xlsx
+++ b/Data/CRMAccuracyData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PUTNAM LAB\Titrator\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB1BEF-260B-4A29-969A-AF2C150B63F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A0F7F3-07E0-4FC5-A53D-C52EBE6DB5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -210,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,8 +370,14 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +557,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -712,7 +724,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,6 +733,12 @@
     <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1076,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="E169" sqref="E169"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="M170" sqref="M170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4462,7 +4480,7 @@
         <v>2224.4699999999998</v>
       </c>
       <c r="D162" s="1">
-        <f t="shared" ref="D162:D167" si="20">100*(B162-C162)/C162</f>
+        <f t="shared" ref="D162:D169" si="20">100*(B162-C162)/C162</f>
         <v>-2.1396062085382019</v>
       </c>
       <c r="E162" s="1">
@@ -4576,6 +4594,57 @@
       <c r="F167" s="1" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="168" spans="1:6" ht="15.6">
+      <c r="A168" s="5">
+        <v>20250819</v>
+      </c>
+      <c r="B168" s="5">
+        <v>2219.70714</v>
+      </c>
+      <c r="C168" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D168" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.21411212558496268</v>
+      </c>
+      <c r="E168" s="1">
+        <v>180</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" ht="15.6">
+      <c r="A169" s="5">
+        <v>20250819</v>
+      </c>
+      <c r="B169" s="5">
+        <v>2213.6607899999999</v>
+      </c>
+      <c r="C169" s="1">
+        <v>2224.4699999999998</v>
+      </c>
+      <c r="D169" s="1">
+        <f t="shared" si="20"/>
+        <v>-0.48592293894725014</v>
+      </c>
+      <c r="E169" s="1">
+        <v>181</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="D172" s="6"/>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="D173" s="6"/>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="D174" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>